<commit_message>
clarify param in table
</commit_message>
<xml_diff>
--- a/Tables_SOS.xlsx
+++ b/Tables_SOS.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17955" windowHeight="9390" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17955" windowHeight="9390" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="1) Lake characteristics" sheetId="1" r:id="rId1"/>
@@ -575,18 +575,12 @@
     <t>Lake surface area</t>
   </si>
   <si>
-    <t>Proportion of catchment with tree cover</t>
-  </si>
-  <si>
     <t>Proportion of lake inflow as groundwater</t>
   </si>
   <si>
     <t>Loading rate of POC from wetlands</t>
   </si>
   <si>
-    <t>Proportion of catchment that is wetlands</t>
-  </si>
-  <si>
     <t>Lake water DOC concentration at start of model run</t>
   </si>
   <si>
@@ -609,6 +603,12 @@
   </si>
   <si>
     <t>Table 5. Model goodness of fit (RMSE, mg/L)</t>
+  </si>
+  <si>
+    <t>Proportion of shoreline with tree cover</t>
+  </si>
+  <si>
+    <t>Proportion of shoreline that is wetlands</t>
   </si>
 </sst>
 </file>
@@ -1093,7 +1093,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1546,8 +1546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="N29" sqref="N29"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1697,7 +1697,7 @@
         <v>123</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C8" s="3">
         <v>3.7</v>
@@ -1720,7 +1720,7 @@
         <v>42</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C9" s="3">
         <v>0.37</v>
@@ -1817,7 +1817,7 @@
         <v>37</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="C15" s="3">
         <v>1</v>
@@ -1840,7 +1840,7 @@
         <v>38</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="C16" s="3">
         <v>0</v>
@@ -1863,7 +1863,7 @@
         <v>47</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C17" s="3">
         <v>1</v>
@@ -1886,7 +1886,7 @@
         <v>125</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C18" s="3">
         <v>10</v>
@@ -1909,7 +1909,7 @@
         <v>39</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C19" s="3">
         <v>0</v>
@@ -1932,7 +1932,7 @@
         <v>48</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C20" s="3">
         <v>2</v>
@@ -2030,7 +2030,7 @@
         <v>46</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C26" s="3">
         <v>1</v>
@@ -2511,7 +2511,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -2519,7 +2519,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" thickBot="1">
       <c r="A1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickBot="1">
@@ -2527,10 +2527,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="42" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C2" s="42" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:3">

</xml_diff>

<commit_message>
update params in table
</commit_message>
<xml_diff>
--- a/Tables_SOS.xlsx
+++ b/Tables_SOS.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="143">
   <si>
     <t>Lake</t>
   </si>
@@ -310,9 +310,6 @@
     <t>PropGW</t>
   </si>
   <si>
-    <t>R_auto</t>
-  </si>
-  <si>
     <t>Parameter</t>
   </si>
   <si>
@@ -616,10 +613,10 @@
     <t>Resp</t>
   </si>
   <si>
-    <t>1- BurialFactor R</t>
-  </si>
-  <si>
-    <t>1- BurialFactor L</t>
+    <t>Leaching rate of POC to DOC (1- BurialFactor R)</t>
+  </si>
+  <si>
+    <t>Leaching rate of POC to DOC (1- BurialFactor L)</t>
   </si>
 </sst>
 </file>
@@ -699,7 +696,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -709,12 +706,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -751,7 +742,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -823,11 +814,9 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -843,7 +832,6 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1161,10 +1149,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>32</v>
@@ -1173,7 +1161,7 @@
         <v>15</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G2" s="9" t="s">
         <v>16</v>
@@ -1188,13 +1176,13 @@
         <v>20</v>
       </c>
       <c r="K2" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N2" s="10" t="s">
         <v>19</v>
@@ -1214,10 +1202,10 @@
         <v>5</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>35</v>
@@ -1264,16 +1252,16 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4" s="14" t="s">
         <v>64</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="C4" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="D4" s="14" t="s">
-        <v>65</v>
       </c>
       <c r="E4" s="15">
         <v>1326</v>
@@ -1312,7 +1300,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C5" s="14" t="s">
         <v>29</v>
@@ -1365,10 +1353,10 @@
         <v>1</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>33</v>
@@ -1418,7 +1406,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C7" s="21" t="s">
         <v>28</v>
@@ -1459,12 +1447,12 @@
       <c r="Q7" s="24"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="39" t="s">
+      <c r="A10" s="37" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:17" ht="13" x14ac:dyDescent="0.25">
-      <c r="A11" s="40" t="s">
+      <c r="A11" s="38" t="s">
         <v>6</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -1473,14 +1461,14 @@
       <c r="C11" s="1"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="40" t="s">
+      <c r="A12" s="38" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
     </row>
     <row r="13" spans="1:17" ht="13" x14ac:dyDescent="0.25">
-      <c r="A13" s="40" t="s">
+      <c r="A13" s="38" t="s">
         <v>5</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -1489,7 +1477,7 @@
       <c r="C13" s="1"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="40" t="s">
+      <c r="A14" s="38" t="s">
         <v>7</v>
       </c>
       <c r="B14" s="4" t="s">
@@ -1497,23 +1485,23 @@
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="40" t="s">
+      <c r="A15" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="B15" s="40" t="s">
+      <c r="B15" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="40"/>
+      <c r="C15" s="38"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="40" t="s">
+      <c r="A16" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="40"/>
-      <c r="C16" s="40"/>
+      <c r="B16" s="38"/>
+      <c r="C16" s="38"/>
     </row>
     <row r="17" spans="1:3" ht="13" x14ac:dyDescent="0.25">
-      <c r="A17" s="40" t="s">
+      <c r="A17" s="38" t="s">
         <v>3</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -1522,14 +1510,14 @@
       <c r="C17" s="1"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="40"/>
+      <c r="A18" s="38"/>
       <c r="B18" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C18" s="1"/>
     </row>
     <row r="19" spans="1:3" ht="13" x14ac:dyDescent="0.25">
-      <c r="A19" s="40" t="s">
+      <c r="A19" s="38" t="s">
         <v>1</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -1538,25 +1526,25 @@
       <c r="C19" s="1"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="40" t="s">
+      <c r="A20" s="38" t="s">
         <v>4</v>
       </c>
       <c r="B20" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20" s="2"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="38" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="38" t="s">
         <v>63</v>
       </c>
-      <c r="C20" s="2"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="40" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="40" t="s">
-        <v>64</v>
-      </c>
       <c r="B22" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1567,16 +1555,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.26953125" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.81640625" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="12.26953125" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.453125" style="3" bestFit="1" customWidth="1"/>
@@ -1586,21 +1574,21 @@
   <sheetData>
     <row r="1" spans="1:7" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>3</v>
@@ -1614,7 +1602,7 @@
     </row>
     <row r="3" spans="1:7" ht="13" x14ac:dyDescent="0.3">
       <c r="A3" s="27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B3" s="27"/>
       <c r="C3" s="28"/>
@@ -1628,7 +1616,7 @@
         <v>16</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C4" s="3">
         <v>4000</v>
@@ -1651,7 +1639,7 @@
         <v>17</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C5" s="3">
         <v>12</v>
@@ -1671,10 +1659,10 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C6" s="3">
         <v>713800</v>
@@ -1694,10 +1682,10 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C7" s="3">
         <v>8320000</v>
@@ -1717,10 +1705,10 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C8" s="3">
         <v>3.7</v>
@@ -1740,10 +1728,10 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C9" s="3">
         <v>0.37</v>
@@ -1763,13 +1751,13 @@
     </row>
     <row r="10" spans="1:7" ht="13" x14ac:dyDescent="0.3">
       <c r="A10" s="27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B10" s="27"/>
     </row>
     <row r="11" spans="1:7" ht="13" x14ac:dyDescent="0.3">
       <c r="A11" s="30" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B11" s="30"/>
       <c r="C11" s="30">
@@ -1790,7 +1778,7 @@
     </row>
     <row r="12" spans="1:7" ht="13" x14ac:dyDescent="0.3">
       <c r="A12" s="30" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B12" s="30"/>
       <c r="C12" s="30">
@@ -1811,7 +1799,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C13" s="3">
         <v>78</v>
@@ -1831,7 +1819,7 @@
     </row>
     <row r="14" spans="1:7" ht="13" x14ac:dyDescent="0.3">
       <c r="A14" s="27" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B14" s="27"/>
     </row>
@@ -1840,7 +1828,7 @@
         <v>37</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C15" s="3">
         <v>1</v>
@@ -1863,7 +1851,7 @@
         <v>38</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C16" s="3">
         <v>0</v>
@@ -1883,10 +1871,10 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C17" s="3">
         <v>1</v>
@@ -1906,10 +1894,10 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C18" s="3">
         <v>10</v>
@@ -1932,7 +1920,7 @@
         <v>39</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C19" s="3">
         <v>0</v>
@@ -1952,10 +1940,10 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C20" s="3">
         <v>2</v>
@@ -1975,13 +1963,13 @@
     </row>
     <row r="21" spans="1:7" ht="13" x14ac:dyDescent="0.3">
       <c r="A21" s="27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B21" s="27"/>
     </row>
     <row r="22" spans="1:7" ht="13" x14ac:dyDescent="0.3">
       <c r="A22" s="30" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B22" s="30"/>
       <c r="C22" s="30">
@@ -2002,7 +1990,7 @@
     </row>
     <row r="23" spans="1:7" ht="13" x14ac:dyDescent="0.3">
       <c r="A23" s="30" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B23" s="30"/>
       <c r="C23" s="30">
@@ -2023,106 +2011,85 @@
     </row>
     <row r="24" spans="1:7" ht="13" x14ac:dyDescent="0.3">
       <c r="A24" s="33" t="s">
-        <v>40</v>
+        <v>76</v>
       </c>
       <c r="B24" s="33"/>
-      <c r="C24" s="47">
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C25" s="3">
         <v>1</v>
       </c>
-      <c r="D24" s="47">
-        <v>0.81556714708038602</v>
-      </c>
-      <c r="E24" s="47">
-        <v>1.0697000000000001</v>
-      </c>
-      <c r="F24" s="47">
-        <v>0.70738097645393605</v>
-      </c>
-      <c r="G24" s="47">
-        <v>0.55418524872402897</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="13" x14ac:dyDescent="0.3">
-      <c r="A25" s="34" t="s">
-        <v>77</v>
-      </c>
-      <c r="B25" s="34"/>
+      <c r="D25" s="3">
+        <v>1</v>
+      </c>
+      <c r="E25" s="3">
+        <v>1</v>
+      </c>
+      <c r="F25" s="3">
+        <v>1</v>
+      </c>
+      <c r="G25" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>46</v>
+        <v>68</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="C26" s="3">
-        <v>1</v>
-      </c>
-      <c r="D26" s="3">
-        <v>1</v>
-      </c>
-      <c r="E26" s="3">
-        <v>1</v>
-      </c>
-      <c r="F26" s="3">
-        <v>1</v>
-      </c>
-      <c r="G26" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="13" x14ac:dyDescent="0.3">
-      <c r="A27" s="30" t="s">
-        <v>69</v>
-      </c>
-      <c r="B27" s="30" t="s">
-        <v>142</v>
-      </c>
-      <c r="C27" s="30">
         <f>1-C11</f>
         <v>2.5000000000000022E-2</v>
       </c>
-      <c r="D27" s="30">
+      <c r="D26" s="3">
         <f>1-D11</f>
         <v>6.4999999999999947E-2</v>
       </c>
-      <c r="E27" s="30">
-        <f t="shared" ref="D27:G27" si="0">1-E11</f>
+      <c r="E26" s="3">
+        <f t="shared" ref="E26:G26" si="0">1-E11</f>
         <v>0.91300000000000003</v>
       </c>
-      <c r="F27" s="30">
+      <c r="F26" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G27" s="30">
+      <c r="G26" s="3">
         <f t="shared" si="0"/>
         <v>8.0000000000002292E-4</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="35" t="s">
-        <v>70</v>
-      </c>
-      <c r="B28" s="35" t="s">
-        <v>143</v>
-      </c>
-      <c r="C28" s="35">
+    <row r="27" spans="1:7" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="B27" s="26" t="s">
+        <v>142</v>
+      </c>
+      <c r="C27" s="26">
         <f>1-C12</f>
         <v>0.99990000000000001</v>
       </c>
-      <c r="D28" s="35">
-        <f t="shared" ref="D28:G28" si="1">1-D12</f>
+      <c r="D27" s="26">
+        <f t="shared" ref="D27:G27" si="1">1-D12</f>
         <v>1.0000000000000009E-3</v>
       </c>
-      <c r="E28" s="35">
+      <c r="E27" s="26">
         <f t="shared" si="1"/>
         <v>0.10099999999999998</v>
       </c>
-      <c r="F28" s="35">
+      <c r="F27" s="26">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="G28" s="35">
+      <c r="G27" s="26">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2148,251 +2115,251 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B1" s="3"/>
     </row>
     <row r="2" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>79</v>
-      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="34" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="34" t="s">
         <v>86</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="36" t="s">
+      <c r="B4" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="34" t="s">
         <v>87</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" s="36" t="s">
+      <c r="B5" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" s="34" t="s">
+        <v>89</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" s="36" t="s">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" s="34" t="s">
         <v>90</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" s="36" t="s">
+      <c r="B7" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" s="34" t="s">
         <v>91</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" s="36" t="s">
+      <c r="B8" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" s="36" t="s">
+      <c r="B9" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" s="34" t="s">
         <v>93</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" s="36" t="s">
-        <v>94</v>
-      </c>
       <c r="B10" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B11" s="27"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="B14" s="3"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" s="34" t="s">
+        <v>96</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B14" s="3"/>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A15" s="36" t="s">
-        <v>97</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>96</v>
-      </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A16" s="36" t="s">
-        <v>99</v>
+      <c r="A16" s="34" t="s">
+        <v>98</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="27" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B25" s="3"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="26" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B30" s="26" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A31" s="37" t="s">
-        <v>108</v>
-      </c>
-      <c r="B31" s="38"/>
+      <c r="A31" s="35" t="s">
+        <v>107</v>
+      </c>
+      <c r="B31" s="36"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B32" s="3"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B33" s="3"/>
     </row>
@@ -2405,7 +2372,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
@@ -2416,7 +2383,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -2424,58 +2391,58 @@
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="D2" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>74</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="45">
+      <c r="B3" s="43">
         <v>39.227373772836103</v>
       </c>
-      <c r="C3" s="45">
+      <c r="C3" s="43">
         <v>164.862709470044</v>
       </c>
-      <c r="D3" s="45">
+      <c r="D3" s="43">
         <v>-180.793888356553</v>
       </c>
-      <c r="E3" s="45">
+      <c r="E3" s="43">
         <v>-5.1203661337195303</v>
       </c>
-      <c r="F3" s="45">
+      <c r="F3" s="43">
         <v>-17.131240983258699</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B4" s="45">
+        <v>63</v>
+      </c>
+      <c r="B4" s="43">
         <v>64.278501302969502</v>
       </c>
-      <c r="C4" s="45">
+      <c r="C4" s="43">
         <v>269.946951924453</v>
       </c>
-      <c r="D4" s="45">
+      <c r="D4" s="43">
         <v>-79.5968838414299</v>
       </c>
-      <c r="E4" s="45">
+      <c r="E4" s="43">
         <v>-194.44344124870301</v>
       </c>
-      <c r="F4" s="45">
+      <c r="F4" s="43">
         <v>-61.9847885743524</v>
       </c>
     </row>
@@ -2483,19 +2450,19 @@
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="45">
+      <c r="B5" s="43">
         <v>276.60654954993498</v>
       </c>
-      <c r="C5" s="45">
+      <c r="C5" s="43">
         <v>57.943578254856099</v>
       </c>
-      <c r="D5" s="45">
+      <c r="D5" s="43">
         <v>-69.872074731636701</v>
       </c>
-      <c r="E5" s="45">
+      <c r="E5" s="43">
         <v>-31.327246220241701</v>
       </c>
-      <c r="F5" s="45">
+      <c r="F5" s="43">
         <v>-232.42809320045399</v>
       </c>
     </row>
@@ -2503,19 +2470,19 @@
       <c r="A6" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="45">
+      <c r="B6" s="43">
         <v>13.7672205375657</v>
       </c>
-      <c r="C6" s="45">
+      <c r="C6" s="43">
         <v>148.46967074848601</v>
       </c>
-      <c r="D6" s="45">
+      <c r="D6" s="43">
         <v>-155.832698328558</v>
       </c>
-      <c r="E6" s="45">
+      <c r="E6" s="43">
         <v>-1.2121897918037099</v>
       </c>
-      <c r="F6" s="45">
+      <c r="F6" s="43">
         <v>-4.6179971627971099</v>
       </c>
     </row>
@@ -2523,19 +2490,19 @@
       <c r="A7" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="46">
+      <c r="B7" s="44">
         <v>40.946599811276002</v>
       </c>
-      <c r="C7" s="46">
+      <c r="C7" s="44">
         <v>134.34037395489801</v>
       </c>
-      <c r="D7" s="46">
+      <c r="D7" s="44">
         <v>-71.806900482945693</v>
       </c>
-      <c r="E7" s="46">
+      <c r="E7" s="44">
         <v>-90.760711309421396</v>
       </c>
-      <c r="F7" s="46">
+      <c r="F7" s="44">
         <v>-12.8955132853542</v>
       </c>
     </row>
@@ -2557,39 +2524,39 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="40" t="s">
+        <v>134</v>
+      </c>
+      <c r="C2" s="40" t="s">
         <v>135</v>
-      </c>
-      <c r="C2" s="42" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="43">
+      <c r="B3" s="41">
         <v>0.55000000000000004</v>
       </c>
-      <c r="C3" s="43">
+      <c r="C3" s="41">
         <v>1.57</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>64</v>
-      </c>
-      <c r="B4" s="43">
+        <v>63</v>
+      </c>
+      <c r="B4" s="41">
         <v>0.72</v>
       </c>
-      <c r="C4" s="43">
+      <c r="C4" s="41">
         <v>1.84</v>
       </c>
     </row>
@@ -2597,10 +2564,10 @@
       <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="43">
+      <c r="B5" s="41">
         <v>3.83</v>
       </c>
-      <c r="C5" s="43">
+      <c r="C5" s="41">
         <v>1.36</v>
       </c>
     </row>
@@ -2608,21 +2575,21 @@
       <c r="A6" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="43">
+      <c r="B6" s="41">
         <v>0.61</v>
       </c>
-      <c r="C6" s="43">
+      <c r="C6" s="41">
         <v>0.87</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="41" t="s">
+      <c r="A7" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="44">
+      <c r="B7" s="42">
         <v>0.33</v>
       </c>
-      <c r="C7" s="44">
+      <c r="C7" s="42">
         <v>0.98</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update param descriptions in table
</commit_message>
<xml_diff>
--- a/Tables_SOS.xlsx
+++ b/Tables_SOS.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="145">
   <si>
     <t>Lake</t>
   </si>
@@ -617,6 +617,12 @@
   </si>
   <si>
     <t>Leaching rate of POC to DOC (1- BurialFactor L)</t>
+  </si>
+  <si>
+    <t>Heterotrophic respiration</t>
+  </si>
+  <si>
+    <t>Proportion of POC buried in sediments</t>
   </si>
 </sst>
 </file>
@@ -1557,8 +1563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:XFD23"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1759,7 +1765,9 @@
       <c r="A11" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="B11" s="30"/>
+      <c r="B11" s="30" t="s">
+        <v>144</v>
+      </c>
       <c r="C11" s="30">
         <v>0.97499999999999998</v>
       </c>
@@ -1780,7 +1788,9 @@
       <c r="A12" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="B12" s="30"/>
+      <c r="B12" s="30" t="s">
+        <v>144</v>
+      </c>
       <c r="C12" s="30">
         <v>1E-4</v>
       </c>
@@ -1971,7 +1981,9 @@
       <c r="A22" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="B22" s="30"/>
+      <c r="B22" s="30" t="s">
+        <v>143</v>
+      </c>
       <c r="C22" s="30">
         <v>1.9E-3</v>
       </c>
@@ -1992,7 +2004,9 @@
       <c r="A23" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="B23" s="30"/>
+      <c r="B23" s="30" t="s">
+        <v>143</v>
+      </c>
       <c r="C23" s="30">
         <v>9.9900000000000003E-2</v>
       </c>

</xml_diff>

<commit_message>
includes new fate means
</commit_message>
<xml_diff>
--- a/Tables_SOS.xlsx
+++ b/Tables_SOS.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17766"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17960" windowHeight="9390" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17960" windowHeight="9390" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="1) Lake characteristics" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="149">
   <si>
     <t>Lake</t>
   </si>
@@ -623,6 +623,18 @@
   </si>
   <si>
     <t>Proportion of POC buried in sediments</t>
+  </si>
+  <si>
+    <t>R_auto</t>
+  </si>
+  <si>
+    <t>Proportion of GPP autotrophically respired</t>
+  </si>
+  <si>
+    <t>Total Load</t>
+  </si>
+  <si>
+    <t>proportion of total load</t>
   </si>
 </sst>
 </file>
@@ -748,7 +760,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -838,6 +850,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1561,10 +1574,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView topLeftCell="A13" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -2023,87 +2036,110 @@
         <v>8.9200000000000002E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="13" x14ac:dyDescent="0.3">
-      <c r="A24" s="33" t="s">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C24" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="D24" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="E24" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="F24" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="G24" s="3">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+      <c r="A25" s="33" t="s">
         <v>76</v>
       </c>
-      <c r="B24" s="33"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="C25" s="3">
-        <v>1</v>
-      </c>
-      <c r="D25" s="3">
-        <v>1</v>
-      </c>
-      <c r="E25" s="3">
-        <v>1</v>
-      </c>
-      <c r="F25" s="3">
-        <v>1</v>
-      </c>
-      <c r="G25" s="3">
-        <v>1</v>
-      </c>
+      <c r="B25" s="33"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C26" s="3">
+        <v>1</v>
+      </c>
+      <c r="D26" s="3">
+        <v>1</v>
+      </c>
+      <c r="E26" s="3">
+        <v>1</v>
+      </c>
+      <c r="F26" s="3">
+        <v>1</v>
+      </c>
+      <c r="G26" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B27" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="C26" s="3">
+      <c r="C27" s="3">
         <f>1-C11</f>
         <v>2.5000000000000022E-2</v>
       </c>
-      <c r="D26" s="3">
+      <c r="D27" s="3">
         <f>1-D11</f>
         <v>6.4999999999999947E-2</v>
       </c>
-      <c r="E26" s="3">
-        <f t="shared" ref="E26:G26" si="0">1-E11</f>
+      <c r="E27" s="3">
+        <f t="shared" ref="E27:G27" si="0">1-E11</f>
         <v>0.91300000000000003</v>
       </c>
-      <c r="F26" s="3">
+      <c r="F27" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G26" s="3">
+      <c r="G27" s="3">
         <f t="shared" si="0"/>
         <v>8.0000000000002292E-4</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="13" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="26" t="s">
+    <row r="28" spans="1:7" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="B27" s="26" t="s">
+      <c r="B28" s="26" t="s">
         <v>142</v>
       </c>
-      <c r="C27" s="26">
+      <c r="C28" s="26">
         <f>1-C12</f>
         <v>0.99990000000000001</v>
       </c>
-      <c r="D27" s="26">
-        <f t="shared" ref="D27:G27" si="1">1-D12</f>
+      <c r="D28" s="26">
+        <f t="shared" ref="D28:G28" si="1">1-D12</f>
         <v>1.0000000000000009E-3</v>
       </c>
-      <c r="E27" s="26">
+      <c r="E28" s="26">
         <f t="shared" si="1"/>
         <v>0.10099999999999998</v>
       </c>
-      <c r="F27" s="26">
+      <c r="F28" s="26">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="G27" s="26">
+      <c r="G28" s="26">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -2118,8 +2154,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B33"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2384,23 +2420,25 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.1796875" style="3"/>
+    <col min="1" max="6" width="9.1796875" style="3"/>
+    <col min="7" max="7" width="10" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.1796875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -2419,28 +2457,35 @@
       <c r="F2" s="6" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" s="12" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="43">
-        <v>39.227373772836103</v>
+        <v>39.227373665459403</v>
       </c>
       <c r="C3" s="43">
-        <v>164.862709470044</v>
+        <v>32.972541848402997</v>
       </c>
       <c r="D3" s="43">
-        <v>-180.793888356553</v>
+        <v>-49.361781911712903</v>
       </c>
       <c r="E3" s="43">
-        <v>-5.1203661337195303</v>
+        <v>-5.2397218243944401</v>
       </c>
       <c r="F3" s="43">
-        <v>-17.131240983258699</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>-16.721576535678501</v>
+      </c>
+      <c r="G3" s="43">
+        <f>SUM(B3:C3)</f>
+        <v>72.199915513862408</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>63</v>
       </c>
@@ -2448,19 +2493,23 @@
         <v>64.278501302969502</v>
       </c>
       <c r="C4" s="43">
-        <v>269.946951924453</v>
+        <v>53.989390405054699</v>
       </c>
       <c r="D4" s="43">
-        <v>-79.5968838414299</v>
+        <v>-17.159384359355801</v>
       </c>
       <c r="E4" s="43">
-        <v>-194.44344124870301</v>
+        <v>-43.559271034049203</v>
       </c>
       <c r="F4" s="43">
-        <v>-61.9847885743524</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>-59.441311511547198</v>
+      </c>
+      <c r="G4" s="43">
+        <f t="shared" ref="G4:G7" si="0">SUM(B4:C4)</f>
+        <v>118.26789170802419</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -2468,56 +2517,231 @@
         <v>276.60654954993498</v>
       </c>
       <c r="C5" s="43">
-        <v>57.943578254856099</v>
+        <v>11.5887156496491</v>
       </c>
       <c r="D5" s="43">
-        <v>-69.872074731636701</v>
+        <v>-97.681533870314794</v>
       </c>
       <c r="E5" s="43">
-        <v>-31.327246220241701</v>
+        <v>-19.542049397210601</v>
       </c>
       <c r="F5" s="43">
-        <v>-232.42809320045399</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>-172.326708872983</v>
+      </c>
+      <c r="G5" s="43">
+        <f t="shared" si="0"/>
+        <v>288.19526519958407</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="43">
-        <v>13.7672205375657</v>
+        <v>13.7672204784194</v>
       </c>
       <c r="C6" s="43">
-        <v>148.46967074848601</v>
+        <v>29.693934144166601</v>
       </c>
       <c r="D6" s="43">
-        <v>-155.832698328558</v>
+        <v>-38.167353667255803</v>
       </c>
       <c r="E6" s="43">
-        <v>-1.2121897918037099</v>
+        <v>-1.2416790147502399</v>
       </c>
       <c r="F6" s="43">
-        <v>-4.6179971627971099</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+        <v>-4.0844277396896604</v>
+      </c>
+      <c r="G6" s="43">
+        <f t="shared" si="0"/>
+        <v>43.461154622586001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="26" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="44">
-        <v>40.946599811276002</v>
+        <v>40.946599812544498</v>
       </c>
       <c r="C7" s="44">
-        <v>134.34037395489801</v>
+        <v>26.868074764514802</v>
       </c>
       <c r="D7" s="44">
-        <v>-71.806900482945693</v>
+        <v>-35.3411046102173</v>
       </c>
       <c r="E7" s="44">
-        <v>-90.760711309421396</v>
+        <v>-20.5409199346328</v>
       </c>
       <c r="F7" s="44">
-        <v>-12.8955132853542</v>
+        <v>-12.472627737519201</v>
+      </c>
+      <c r="G7" s="44">
+        <f t="shared" si="0"/>
+        <v>67.814674577059293</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="B9"/>
+      <c r="C9"/>
+      <c r="D9"/>
+      <c r="E9"/>
+      <c r="F9"/>
+    </row>
+    <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B10"/>
+      <c r="C10"/>
+      <c r="D10"/>
+      <c r="E10"/>
+      <c r="F10"/>
+    </row>
+    <row r="11" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="G11" s="45"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="43">
+        <f>B3/$G$3</f>
+        <v>0.54331606050048264</v>
+      </c>
+      <c r="C12" s="43">
+        <f t="shared" ref="C12:F12" si="1">C3/$G$3</f>
+        <v>0.45668393949951724</v>
+      </c>
+      <c r="D12" s="43">
+        <f t="shared" si="1"/>
+        <v>-0.68368198993578355</v>
+      </c>
+      <c r="E12" s="43">
+        <f t="shared" si="1"/>
+        <v>-7.2572409359515269E-2</v>
+      </c>
+      <c r="F12" s="43">
+        <f t="shared" si="1"/>
+        <v>-0.23160105405480638</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13" s="43">
+        <f>B4/$G$4</f>
+        <v>0.54349917272270409</v>
+      </c>
+      <c r="C13" s="43">
+        <f>C4/$G$4</f>
+        <v>0.45650082727729596</v>
+      </c>
+      <c r="D13" s="43">
+        <f>D4/$G$4</f>
+        <v>-0.14508912022984491</v>
+      </c>
+      <c r="E13" s="43">
+        <f t="shared" ref="D13:F13" si="2">E4/$G$4</f>
+        <v>-0.36831020156837557</v>
+      </c>
+      <c r="F13" s="43">
+        <f t="shared" si="2"/>
+        <v>-0.50259889352127718</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="43">
+        <f>B5/$G$5</f>
+        <v>0.95978866744523528</v>
+      </c>
+      <c r="C14" s="43">
+        <f t="shared" ref="C14:F14" si="3">C5/$G$5</f>
+        <v>4.0211332554764764E-2</v>
+      </c>
+      <c r="D14" s="43">
+        <f t="shared" si="3"/>
+        <v>-0.33894218838976181</v>
+      </c>
+      <c r="E14" s="43">
+        <f t="shared" si="3"/>
+        <v>-6.780836383164425E-2</v>
+      </c>
+      <c r="F14" s="43">
+        <f t="shared" si="3"/>
+        <v>-0.59795121461708078</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="43">
+        <f>B6/$G$6</f>
+        <v>0.31677070243469363</v>
+      </c>
+      <c r="C15" s="43">
+        <f t="shared" ref="C15:F15" si="4">C6/$G$6</f>
+        <v>0.68322929756530637</v>
+      </c>
+      <c r="D15" s="43">
+        <f t="shared" si="4"/>
+        <v>-0.87819465448395839</v>
+      </c>
+      <c r="E15" s="43">
+        <f t="shared" si="4"/>
+        <v>-2.856985796932696E-2</v>
+      </c>
+      <c r="F15" s="43">
+        <f t="shared" si="4"/>
+        <v>-9.397881338309072E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="44">
+        <f t="shared" ref="B16:F16" si="5">B7/$G$3</f>
+        <v>0.56712808486157773</v>
+      </c>
+      <c r="C16" s="44">
+        <f t="shared" si="5"/>
+        <v>0.37213443496836396</v>
+      </c>
+      <c r="D16" s="44">
+        <f t="shared" si="5"/>
+        <v>-0.48948955630608454</v>
+      </c>
+      <c r="E16" s="44">
+        <f t="shared" si="5"/>
+        <v>-0.28450060901648749</v>
+      </c>
+      <c r="F16" s="44">
+        <f t="shared" si="5"/>
+        <v>-0.17275127884497943</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update complete cases for rmse
</commit_message>
<xml_diff>
--- a/Tables_SOS.xlsx
+++ b/Tables_SOS.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17960" windowHeight="9390" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17960" windowHeight="9390" firstSheet="3" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="1) Lake characteristics" sheetId="1" r:id="rId1"/>
@@ -2154,7 +2154,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
@@ -2661,7 +2661,7 @@
         <v>-0.14508912022984491</v>
       </c>
       <c r="E13" s="43">
-        <f t="shared" ref="D13:F13" si="2">E4/$G$4</f>
+        <f t="shared" ref="E13:F13" si="2">E4/$G$4</f>
         <v>-0.36831020156837557</v>
       </c>
       <c r="F13" s="43">
@@ -2754,8 +2754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2784,7 +2784,7 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="C3" s="41">
-        <v>1.57</v>
+        <v>1.52</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -2792,10 +2792,10 @@
         <v>63</v>
       </c>
       <c r="B4" s="41">
-        <v>0.72</v>
+        <v>0.68</v>
       </c>
       <c r="C4" s="41">
-        <v>1.84</v>
+        <v>1.75</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -2803,10 +2803,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="41">
-        <v>3.83</v>
+        <v>2.39</v>
       </c>
       <c r="C5" s="41">
-        <v>1.36</v>
+        <v>1.18</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -2814,10 +2814,10 @@
         <v>1</v>
       </c>
       <c r="B6" s="41">
-        <v>0.61</v>
+        <v>0.47</v>
       </c>
       <c r="C6" s="41">
-        <v>0.87</v>
+        <v>0.76</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2825,10 +2825,10 @@
         <v>4</v>
       </c>
       <c r="B7" s="42">
-        <v>0.33</v>
+        <v>0.3</v>
       </c>
       <c r="C7" s="42">
-        <v>0.98</v>
+        <v>0.99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated oxygen flux equations in Tables_SOS
</commit_message>
<xml_diff>
--- a/Tables_SOS.xlsx
+++ b/Tables_SOS.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17830"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\immcc\Desktop\SOS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hdugan\Documents\Rpackages\SOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17960" windowHeight="9390" firstSheet="3" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17955" windowHeight="9390" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="1) Lake characteristics" sheetId="1" r:id="rId1"/>
     <sheet name="2) Model parameters" sheetId="2" r:id="rId2"/>
-    <sheet name="3) Built model with equations" sheetId="3" r:id="rId3"/>
+    <sheet name="3)Equations" sheetId="3" r:id="rId3"/>
     <sheet name="4) Mass balances" sheetId="4" r:id="rId4"/>
     <sheet name="5) RMSE" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="153">
   <si>
     <t>Lake</t>
   </si>
@@ -532,18 +532,6 @@
     <t>Respiration_R = GPP DOC rate * DOCR_RespParam(1.08^(epilimnion temp - 20))</t>
   </si>
   <si>
-    <t>NPP POC_L = GPP POC_L * (1-R_auto) * Area / 1000</t>
-  </si>
-  <si>
-    <t>NPP DOC_L = GPP DOC_L * (1-R_auto) * Area / 1000</t>
-  </si>
-  <si>
-    <t>GPP POC_L rate = GPP POC rate + GPP DOC rate</t>
-  </si>
-  <si>
-    <t>GPP DOC_L rate = 0</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -635,6 +623,30 @@
   </si>
   <si>
     <t>proportion of total load</t>
+  </si>
+  <si>
+    <t>NEP and Oxygen Flux</t>
+  </si>
+  <si>
+    <t>Fatm = 0.7 * (DOconc - DOsat)/Zmix</t>
+  </si>
+  <si>
+    <t>DO(t+1) = DOconc + NEP - Fatm</t>
+  </si>
+  <si>
+    <t>NEP (as O2) = (NPP - DOCrespired) * 32/12</t>
+  </si>
+  <si>
+    <t>g O2/m3</t>
+  </si>
+  <si>
+    <t>g O2/m2</t>
+  </si>
+  <si>
+    <t>NPP DOC_L = GPP DOC_L * 0.2 * Area / 1000</t>
+  </si>
+  <si>
+    <t>NPP POC_L = GPP POC_L * 0.2 * Area / 1000</t>
   </si>
 </sst>
 </file>
@@ -1137,33 +1149,33 @@
       <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.54296875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="15.54296875" style="4" customWidth="1"/>
-    <col min="3" max="3" width="13.453125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7265625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" style="3" customWidth="1"/>
     <col min="5" max="5" width="7" style="3" customWidth="1"/>
-    <col min="6" max="6" width="9.54296875" style="3" customWidth="1"/>
-    <col min="7" max="7" width="9.7265625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="9.54296875" style="4" customWidth="1"/>
-    <col min="9" max="9" width="11.453125" style="3" customWidth="1"/>
-    <col min="10" max="10" width="11.26953125" style="3" customWidth="1"/>
-    <col min="11" max="11" width="7.1796875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="9.5703125" style="4" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" style="3" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" style="3" customWidth="1"/>
     <col min="12" max="12" width="6" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.7265625" style="3" customWidth="1"/>
-    <col min="14" max="14" width="24.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="8.81640625" style="3"/>
+    <col min="13" max="13" width="6.7109375" style="3" customWidth="1"/>
+    <col min="14" max="14" width="24.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="8.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="12" customFormat="1" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" s="12" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -1216,7 +1228,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
         <v>5</v>
       </c>
@@ -1269,7 +1281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
         <v>63</v>
       </c>
@@ -1314,7 +1326,7 @@
       <c r="P4" s="17"/>
       <c r="Q4" s="17"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
         <v>3</v>
       </c>
@@ -1367,7 +1379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
         <v>1</v>
       </c>
@@ -1420,7 +1432,7 @@
         <v>2.9999999999999997E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:17" s="26" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" s="26" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>4</v>
       </c>
@@ -1465,12 +1477,12 @@
       <c r="P7" s="24"/>
       <c r="Q7" s="24"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="37" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="38" t="s">
         <v>6</v>
       </c>
@@ -1479,14 +1491,14 @@
       </c>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="38" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:17" ht="13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="38" t="s">
         <v>5</v>
       </c>
@@ -1495,7 +1507,7 @@
       </c>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="38" t="s">
         <v>7</v>
       </c>
@@ -1503,7 +1515,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="38" t="s">
         <v>2</v>
       </c>
@@ -1512,14 +1524,14 @@
       </c>
       <c r="C15" s="38"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="38" t="s">
         <v>12</v>
       </c>
       <c r="B16" s="38"/>
       <c r="C16" s="38"/>
     </row>
-    <row r="17" spans="1:3" ht="13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="38" t="s">
         <v>3</v>
       </c>
@@ -1528,14 +1540,14 @@
       </c>
       <c r="C17" s="1"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="38"/>
       <c r="B18" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="1:3" ht="13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="38" t="s">
         <v>1</v>
       </c>
@@ -1544,7 +1556,7 @@
       </c>
       <c r="C19" s="1"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="38" t="s">
         <v>4</v>
       </c>
@@ -1553,12 +1565,12 @@
       </c>
       <c r="C20" s="2"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="38" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="38" t="s">
         <v>63</v>
       </c>
@@ -1580,28 +1592,28 @@
       <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="27" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.26953125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.81640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="12.26953125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.26953125" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.1796875" style="3"/>
+    <col min="2" max="2" width="43.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="12.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>40</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>5</v>
@@ -1619,7 +1631,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="27" t="s">
         <v>42</v>
       </c>
@@ -1630,12 +1642,12 @@
       <c r="F3" s="28"/>
       <c r="G3" s="28"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C4" s="3">
         <v>4000</v>
@@ -1653,12 +1665,12 @@
         <v>2007000</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C5" s="3">
         <v>12</v>
@@ -1676,12 +1688,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C6" s="3">
         <v>713800</v>
@@ -1699,12 +1711,12 @@
         <v>5650000000</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>57</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C7" s="3">
         <v>8320000</v>
@@ -1722,12 +1734,12 @@
         <v>153000000000</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C8" s="3">
         <v>3.7</v>
@@ -1745,12 +1757,12 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>41</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C9" s="3">
         <v>0.37</v>
@@ -1768,18 +1780,18 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="27" t="s">
         <v>43</v>
       </c>
       <c r="B10" s="27"/>
     </row>
-    <row r="11" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="30" t="s">
         <v>66</v>
       </c>
       <c r="B11" s="30" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C11" s="30">
         <v>0.97499999999999998</v>
@@ -1797,12 +1809,12 @@
         <v>0.99919999999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="30" t="s">
         <v>67</v>
       </c>
       <c r="B12" s="30" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C12" s="30">
         <v>1E-4</v>
@@ -1820,9 +1832,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C13" s="3">
         <v>78</v>
@@ -1840,18 +1852,18 @@
         <v>186</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="27" t="s">
         <v>77</v>
       </c>
       <c r="B14" s="27"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>37</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C15" s="3">
         <v>1</v>
@@ -1869,12 +1881,12 @@
         <v>0.61470000000000002</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>38</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C16" s="3">
         <v>0</v>
@@ -1892,12 +1904,12 @@
         <v>3.6999999999999998E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C17" s="3">
         <v>1</v>
@@ -1915,12 +1927,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C18" s="3">
         <v>10</v>
@@ -1938,12 +1950,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>39</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C19" s="3">
         <v>0</v>
@@ -1961,12 +1973,12 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>47</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="C20" s="3">
         <v>2</v>
@@ -1984,18 +1996,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="27" t="s">
         <v>44</v>
       </c>
       <c r="B21" s="27"/>
     </row>
-    <row r="22" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="30" t="s">
         <v>70</v>
       </c>
       <c r="B22" s="30" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C22" s="30">
         <v>1.9E-3</v>
@@ -2013,12 +2025,12 @@
         <v>1.1999999999999999E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="30" t="s">
         <v>71</v>
       </c>
       <c r="B23" s="30" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C23" s="30">
         <v>9.9900000000000003E-2</v>
@@ -2036,12 +2048,12 @@
         <v>8.9200000000000002E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C24" s="3">
         <v>0.8</v>
@@ -2059,18 +2071,18 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="33" t="s">
         <v>76</v>
       </c>
       <c r="B25" s="33"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>45</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C26" s="3">
         <v>1</v>
@@ -2088,12 +2100,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>68</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C27" s="3">
         <f>1-C11</f>
@@ -2116,12 +2128,12 @@
         <v>8.0000000000002292E-4</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="26" t="s">
         <v>69</v>
       </c>
       <c r="B28" s="26" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C28" s="26">
         <f>1-C12</f>
@@ -2152,24 +2164,24 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B33"/>
+  <dimension ref="A1:B35"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="92.453125" customWidth="1"/>
+    <col min="1" max="1" width="92.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>105</v>
       </c>
       <c r="B1" s="3"/>
     </row>
-    <row r="2" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>77</v>
       </c>
@@ -2177,7 +2189,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="34" t="s">
         <v>85</v>
       </c>
@@ -2185,7 +2197,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="34" t="s">
         <v>86</v>
       </c>
@@ -2193,7 +2205,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="34" t="s">
         <v>87</v>
       </c>
@@ -2201,7 +2213,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="34" t="s">
         <v>89</v>
       </c>
@@ -2209,7 +2221,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="34" t="s">
         <v>90</v>
       </c>
@@ -2217,7 +2229,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="34" t="s">
         <v>91</v>
       </c>
@@ -2225,7 +2237,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="34" t="s">
         <v>92</v>
       </c>
@@ -2233,7 +2245,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="34" t="s">
         <v>93</v>
       </c>
@@ -2241,13 +2253,13 @@
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="27" t="s">
         <v>43</v>
       </c>
       <c r="B11" s="27"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>83</v>
       </c>
@@ -2255,7 +2267,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>81</v>
       </c>
@@ -2263,13 +2275,13 @@
         <v>84</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="27" t="s">
         <v>94</v>
       </c>
       <c r="B14" s="3"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="34" t="s">
         <v>96</v>
       </c>
@@ -2277,7 +2289,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="34" t="s">
         <v>98</v>
       </c>
@@ -2285,7 +2297,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>100</v>
       </c>
@@ -2293,7 +2305,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>102</v>
       </c>
@@ -2301,120 +2313,135 @@
         <v>95</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>117</v>
+        <v>151</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>116</v>
+        <v>152</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A23" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="B23" s="3" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="27" t="s">
+        <v>145</v>
+      </c>
+      <c r="B23" s="3"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>113</v>
+        <v>148</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A25" s="27" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="27" t="s">
         <v>76</v>
       </c>
-      <c r="B25" s="3"/>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A26" s="3" t="s">
+      <c r="B27" s="3"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B28" s="3" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A27" s="3" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
         <v>111</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A28" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A29" s="3" t="s">
-        <v>109</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="26" t="s">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="B30" s="26" t="s">
+      <c r="B32" s="26" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A31" s="35" t="s">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="35" t="s">
         <v>107</v>
       </c>
-      <c r="B31" s="36"/>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A32" s="3" t="s">
+      <c r="B33" s="36"/>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="B32" s="3"/>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A33" s="3" t="s">
+      <c r="B34" s="3"/>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="B33" s="3"/>
+      <c r="B35" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2426,19 +2453,19 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="6" width="9.1796875" style="3"/>
+    <col min="1" max="6" width="9.140625" style="3"/>
     <col min="7" max="7" width="10" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.1796875" style="3"/>
+    <col min="8" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -2449,19 +2476,19 @@
         <v>73</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>74</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
@@ -2485,7 +2512,7 @@
         <v>72.199915513862408</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>63</v>
       </c>
@@ -2509,7 +2536,7 @@
         <v>118.26789170802419</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -2533,7 +2560,7 @@
         <v>288.19526519958407</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>1</v>
       </c>
@@ -2557,7 +2584,7 @@
         <v>43.461154622586001</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
         <v>4</v>
       </c>
@@ -2581,16 +2608,16 @@
         <v>67.814674577059293</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="B9"/>
       <c r="C9"/>
       <c r="D9"/>
       <c r="E9"/>
       <c r="F9"/>
     </row>
-    <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B10"/>
       <c r="C10"/>
@@ -2598,7 +2625,7 @@
       <c r="E10"/>
       <c r="F10"/>
     </row>
-    <row r="11" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>0</v>
       </c>
@@ -2609,17 +2636,17 @@
         <v>73</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>74</v>
       </c>
       <c r="G11" s="45"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>5</v>
       </c>
@@ -2644,7 +2671,7 @@
         <v>-0.23160105405480638</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>63</v>
       </c>
@@ -2669,7 +2696,7 @@
         <v>-0.50259889352127718</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>3</v>
       </c>
@@ -2694,7 +2721,7 @@
         <v>-0.59795121461708078</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>1</v>
       </c>
@@ -2719,7 +2746,7 @@
         <v>-9.397881338309072E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="26" t="s">
         <v>4</v>
       </c>
@@ -2754,29 +2781,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="40" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="40" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C2" s="40" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -2787,7 +2814,7 @@
         <v>1.52</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>63</v>
       </c>
@@ -2798,7 +2825,7 @@
         <v>1.75</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -2809,7 +2836,7 @@
         <v>1.18</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -2820,7 +2847,7 @@
         <v>0.76</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="39" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
update table with new results
</commit_message>
<xml_diff>
--- a/Tables_SOS.xlsx
+++ b/Tables_SOS.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="153">
   <si>
     <t>Lake</t>
   </si>
@@ -644,6 +644,9 @@
   </si>
   <si>
     <t>g O2/m3/d</t>
+  </si>
+  <si>
+    <t>old</t>
   </si>
 </sst>
 </file>
@@ -2447,10 +2450,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -2460,12 +2463,15 @@
     <col min="8" max="16384" width="9.1796875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I1" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -2487,8 +2493,23 @@
       <c r="G2" s="12" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I2" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
@@ -2511,8 +2532,23 @@
         <f>SUM(B3:C3)</f>
         <v>72.199915513862408</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I3" s="43">
+        <v>39.227373665459403</v>
+      </c>
+      <c r="J3" s="43">
+        <v>32.972541848402997</v>
+      </c>
+      <c r="K3" s="43">
+        <v>-49.361781911712903</v>
+      </c>
+      <c r="L3" s="43">
+        <v>-5.2397218243944401</v>
+      </c>
+      <c r="M3" s="43">
+        <v>-16.721576535678501</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>63</v>
       </c>
@@ -2523,68 +2559,113 @@
         <v>53.989390405054699</v>
       </c>
       <c r="D4" s="43">
-        <v>-17.159384359355801</v>
+        <v>-17.2970662136591</v>
       </c>
       <c r="E4" s="43">
-        <v>-43.559271034049203</v>
+        <v>-43.585940747489801</v>
       </c>
       <c r="F4" s="43">
-        <v>-59.441311511547198</v>
+        <v>-59.071439536272599</v>
       </c>
       <c r="G4" s="43">
         <f t="shared" ref="G4:G7" si="0">SUM(B4:C4)</f>
         <v>118.26789170802419</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I4" s="43">
+        <v>64.278501302969502</v>
+      </c>
+      <c r="J4" s="43">
+        <v>53.989390405054699</v>
+      </c>
+      <c r="K4" s="43">
+        <v>-17.159384359355801</v>
+      </c>
+      <c r="L4" s="43">
+        <v>-43.559271034049203</v>
+      </c>
+      <c r="M4" s="43">
+        <v>-59.441311511547198</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="43">
-        <v>276.60654954993498</v>
+        <v>97.128960515597697</v>
       </c>
       <c r="C5" s="43">
         <v>11.5887156496491</v>
       </c>
       <c r="D5" s="43">
-        <v>-97.681533870314794</v>
+        <v>-27.0525356096257</v>
       </c>
       <c r="E5" s="43">
-        <v>-19.542049397210601</v>
+        <v>-13.0780374098991</v>
       </c>
       <c r="F5" s="43">
-        <v>-172.326708872983</v>
+        <v>-67.421687759106604</v>
       </c>
       <c r="G5" s="43">
         <f t="shared" si="0"/>
-        <v>288.19526519958407</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>108.7176761652468</v>
+      </c>
+      <c r="I5" s="43">
+        <v>276.60654954993498</v>
+      </c>
+      <c r="J5" s="43">
+        <v>11.5887156496491</v>
+      </c>
+      <c r="K5" s="43">
+        <v>-97.681533870314794</v>
+      </c>
+      <c r="L5" s="43">
+        <v>-19.542049397210601</v>
+      </c>
+      <c r="M5" s="43">
+        <v>-172.326708872983</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="43">
-        <v>13.7672204784194</v>
+        <v>13.767220528508201</v>
       </c>
       <c r="C6" s="43">
-        <v>29.693934144166601</v>
+        <v>29.6939341325543</v>
       </c>
       <c r="D6" s="43">
-        <v>-38.167353667255803</v>
+        <v>-38.1948755798024</v>
       </c>
       <c r="E6" s="43">
-        <v>-1.2416790147502399</v>
+        <v>-1.2121897918037099</v>
       </c>
       <c r="F6" s="43">
-        <v>-4.0844277396896604</v>
+        <v>-4.1449302423290497</v>
       </c>
       <c r="G6" s="43">
         <f t="shared" si="0"/>
-        <v>43.461154622586001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+        <v>43.461154661062501</v>
+      </c>
+      <c r="I6" s="43">
+        <v>13.7672204784194</v>
+      </c>
+      <c r="J6" s="43">
+        <v>29.693934144166601</v>
+      </c>
+      <c r="K6" s="43">
+        <v>-38.167353667255803</v>
+      </c>
+      <c r="L6" s="43">
+        <v>-1.2416790147502399</v>
+      </c>
+      <c r="M6" s="43">
+        <v>-4.0844277396896604</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="26" t="s">
         <v>4</v>
       </c>
@@ -2607,15 +2688,30 @@
         <f t="shared" si="0"/>
         <v>67.814674577059293</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
+      <c r="I7" s="44">
+        <v>40.946599812544498</v>
+      </c>
+      <c r="J7" s="44">
+        <v>26.868074764514802</v>
+      </c>
+      <c r="K7" s="44">
+        <v>-35.3411046102173</v>
+      </c>
+      <c r="L7" s="44">
+        <v>-20.5409199346328</v>
+      </c>
+      <c r="M7" s="44">
+        <v>-12.472627737519201</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
       <c r="B9"/>
       <c r="C9"/>
       <c r="D9"/>
       <c r="E9"/>
       <c r="F9"/>
     </row>
-    <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="3" t="s">
         <v>143</v>
       </c>
@@ -2625,7 +2721,7 @@
       <c r="E10"/>
       <c r="F10"/>
     </row>
-    <row r="11" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6" t="s">
         <v>0</v>
       </c>
@@ -2646,7 +2742,7 @@
       </c>
       <c r="G11" s="45"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>5</v>
       </c>
@@ -2659,7 +2755,7 @@
         <v>0.45668393949951724</v>
       </c>
       <c r="D12" s="43">
-        <f t="shared" si="1"/>
+        <f>D3/$G$3</f>
         <v>-0.68368198993578355</v>
       </c>
       <c r="E12" s="43">
@@ -2671,7 +2767,7 @@
         <v>-0.23160105405480638</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>63</v>
       </c>
@@ -2680,95 +2776,95 @@
         <v>0.54349917272270409</v>
       </c>
       <c r="C13" s="43">
-        <f>C4/$G$4</f>
+        <f t="shared" ref="C13:F13" si="2">C4/$G$4</f>
         <v>0.45650082727729596</v>
       </c>
       <c r="D13" s="43">
-        <f>D4/$G$4</f>
-        <v>-0.14508912022984491</v>
+        <f t="shared" si="2"/>
+        <v>-0.14625327266644372</v>
       </c>
       <c r="E13" s="43">
-        <f t="shared" ref="E13:F13" si="2">E4/$G$4</f>
-        <v>-0.36831020156837557</v>
+        <f t="shared" si="2"/>
+        <v>-0.36853570413763109</v>
       </c>
       <c r="F13" s="43">
         <f t="shared" si="2"/>
-        <v>-0.50259889352127718</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>-0.49947148531324281</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B14" s="43">
         <f>B5/$G$5</f>
-        <v>0.95978866744523528</v>
+        <v>0.89340541429496079</v>
       </c>
       <c r="C14" s="43">
         <f t="shared" ref="C14:F14" si="3">C5/$G$5</f>
-        <v>4.0211332554764764E-2</v>
+        <v>0.10659458570503921</v>
       </c>
       <c r="D14" s="43">
         <f t="shared" si="3"/>
-        <v>-0.33894218838976181</v>
+        <v>-0.24883290890532703</v>
       </c>
       <c r="E14" s="43">
         <f t="shared" si="3"/>
-        <v>-6.780836383164425E-2</v>
+        <v>-0.12029357020123363</v>
       </c>
       <c r="F14" s="43">
         <f t="shared" si="3"/>
-        <v>-0.59795121461708078</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+        <v>-0.62015387135968725</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B15" s="43">
         <f>B6/$G$6</f>
-        <v>0.31677070243469363</v>
+        <v>0.31677070330674989</v>
       </c>
       <c r="C15" s="43">
         <f t="shared" ref="C15:F15" si="4">C6/$G$6</f>
-        <v>0.68322929756530637</v>
+        <v>0.68322929669325005</v>
       </c>
       <c r="D15" s="43">
         <f t="shared" si="4"/>
-        <v>-0.87819465448395839</v>
+        <v>-0.87882790684394219</v>
       </c>
       <c r="E15" s="43">
         <f t="shared" si="4"/>
-        <v>-2.856985796932696E-2</v>
+        <v>-2.7891338857817527E-2</v>
       </c>
       <c r="F15" s="43">
         <f t="shared" si="4"/>
-        <v>-9.397881338309072E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+        <v>-9.5370918574387412E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="26" t="s">
         <v>4</v>
       </c>
       <c r="B16" s="44">
-        <f t="shared" ref="B16:F16" si="5">B7/$G$3</f>
-        <v>0.56712808486157773</v>
+        <f>B7/$G$7</f>
+        <v>0.60380146432784232</v>
       </c>
       <c r="C16" s="44">
-        <f t="shared" si="5"/>
-        <v>0.37213443496836396</v>
+        <f t="shared" ref="C16:F16" si="5">C7/$G$7</f>
+        <v>0.39619853567215785</v>
       </c>
       <c r="D16" s="44">
         <f t="shared" si="5"/>
-        <v>-0.48948955630608454</v>
+        <v>-0.52114243459294984</v>
       </c>
       <c r="E16" s="44">
         <f t="shared" si="5"/>
-        <v>-0.28450060901648749</v>
+        <v>-0.30289786189701029</v>
       </c>
       <c r="F16" s="44">
         <f t="shared" si="5"/>
-        <v>-0.17275127884497943</v>
+        <v>-0.18392225304194718</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new beard plot, updated fix toolik
</commit_message>
<xml_diff>
--- a/Tables_SOS.xlsx
+++ b/Tables_SOS.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17830"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\immcc\Desktop\SOS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hdugan\Documents\Rpackages\SOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17960" windowHeight="9390" firstSheet="3" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17955" windowHeight="9390"/>
   </bookViews>
   <sheets>
     <sheet name="1) Lake characteristics" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="4) Mass balances" sheetId="4" r:id="rId4"/>
     <sheet name="5) RMSE" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="155">
   <si>
     <t>Lake</t>
   </si>
@@ -337,9 +337,6 @@
     <t>2005-2008_Kling_Toolik_DOC: pulled avg DOC for value in DOC column</t>
   </si>
   <si>
-    <t>TP (g/m³)</t>
-  </si>
-  <si>
     <t>Sweden</t>
   </si>
   <si>
@@ -647,6 +644,15 @@
   </si>
   <si>
     <t>old</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reference </t>
+  </si>
+  <si>
+    <t>TP (mg/m³)</t>
+  </si>
+  <si>
+    <t>ChlA</t>
   </si>
 </sst>
 </file>
@@ -772,7 +778,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -863,6 +869,7 @@
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1143,47 +1150,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q22"/>
+  <dimension ref="A1:R22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.54296875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="15.54296875" style="4" customWidth="1"/>
-    <col min="3" max="3" width="13.453125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7265625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="15.5703125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" style="3" customWidth="1"/>
     <col min="5" max="5" width="7" style="3" customWidth="1"/>
-    <col min="6" max="6" width="9.54296875" style="3" customWidth="1"/>
-    <col min="7" max="7" width="9.7265625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="9.54296875" style="4" customWidth="1"/>
-    <col min="9" max="9" width="11.453125" style="3" customWidth="1"/>
-    <col min="10" max="10" width="11.26953125" style="3" customWidth="1"/>
-    <col min="11" max="11" width="7.1796875" style="3" customWidth="1"/>
-    <col min="12" max="12" width="6" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.7265625" style="3" customWidth="1"/>
-    <col min="14" max="14" width="24.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="8.81640625" style="3"/>
+    <col min="6" max="6" width="9.5703125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="9.5703125" style="4" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" style="3" customWidth="1"/>
+    <col min="11" max="12" width="7.140625" style="3" customWidth="1"/>
+    <col min="13" max="13" width="8.5703125" style="3" customWidth="1"/>
+    <col min="14" max="14" width="6.7109375" style="3" customWidth="1"/>
+    <col min="15" max="15" width="24.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="8.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="12" customFormat="1" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:18" s="12" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>32</v>
@@ -1192,7 +1199,7 @@
         <v>15</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G2" s="9" t="s">
         <v>16</v>
@@ -1207,36 +1214,39 @@
         <v>20</v>
       </c>
       <c r="K2" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="L2" s="7" t="s">
-        <v>49</v>
+        <v>55</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>154</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="N2" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="O2" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="O2" s="11" t="s">
+      <c r="P2" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="P2" s="11" t="s">
+      <c r="Q2" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="Q2" s="11" t="s">
+      <c r="R2" s="11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>35</v>
@@ -1254,7 +1264,7 @@
         <v>12</v>
       </c>
       <c r="I3" s="17">
-        <v>3.1</v>
+        <v>2.5</v>
       </c>
       <c r="J3" s="17" t="s">
         <v>22</v>
@@ -1262,37 +1272,38 @@
       <c r="K3" s="17">
         <v>6.5</v>
       </c>
-      <c r="L3" s="17">
+      <c r="L3" s="17"/>
+      <c r="M3" s="17">
         <v>5</v>
       </c>
-      <c r="M3" s="17">
+      <c r="N3" s="17">
         <v>4</v>
       </c>
-      <c r="N3" s="15">
+      <c r="O3" s="15">
         <v>528.27563249500008</v>
       </c>
-      <c r="O3" s="17">
+      <c r="P3" s="17">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="P3" s="17">
+      <c r="Q3" s="17">
         <v>0.84099999999999997</v>
       </c>
-      <c r="Q3" s="17">
+      <c r="R3" s="17">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" s="14" t="s">
         <v>63</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="C4" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="D4" s="14" t="s">
-        <v>64</v>
       </c>
       <c r="E4" s="15">
         <v>1326</v>
@@ -1307,7 +1318,7 @@
         <v>8.3000000000000007</v>
       </c>
       <c r="I4" s="17">
-        <v>0.91</v>
+        <v>0.76</v>
       </c>
       <c r="J4" s="17" t="s">
         <v>21</v>
@@ -1315,23 +1326,24 @@
       <c r="K4" s="17">
         <v>2.68</v>
       </c>
-      <c r="L4" s="18">
+      <c r="L4" s="17"/>
+      <c r="M4" s="18">
         <v>132.1</v>
       </c>
-      <c r="M4" s="18">
+      <c r="N4" s="18">
         <v>6</v>
       </c>
-      <c r="N4" s="15"/>
-      <c r="O4" s="17"/>
+      <c r="O4" s="15"/>
       <c r="P4" s="17"/>
       <c r="Q4" s="17"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R4" s="17"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C5" s="14" t="s">
         <v>29</v>
@@ -1352,7 +1364,7 @@
         <v>7</v>
       </c>
       <c r="I5" s="17">
-        <v>1</v>
+        <v>0.82899999999999996</v>
       </c>
       <c r="J5" s="17" t="s">
         <v>22</v>
@@ -1360,34 +1372,35 @@
       <c r="K5" s="17">
         <v>4.75</v>
       </c>
-      <c r="L5" s="17">
+      <c r="L5" s="17"/>
+      <c r="M5" s="17">
         <v>2</v>
       </c>
-      <c r="M5" s="19">
+      <c r="N5" s="19">
         <v>5</v>
       </c>
-      <c r="N5" s="15">
+      <c r="O5" s="15">
         <v>6752.4100000000008</v>
       </c>
-      <c r="O5" s="17">
+      <c r="P5" s="17">
         <v>0.504</v>
-      </c>
-      <c r="P5" s="17">
-        <v>0</v>
       </c>
       <c r="Q5" s="17">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R5" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>33</v>
@@ -1405,7 +1418,7 @@
         <v>14.6</v>
       </c>
       <c r="I6" s="17">
-        <v>4.5999999999999996</v>
+        <v>5.9</v>
       </c>
       <c r="J6" s="17" t="s">
         <v>22</v>
@@ -1413,31 +1426,32 @@
       <c r="K6" s="17">
         <v>5.32</v>
       </c>
-      <c r="L6" s="17">
+      <c r="L6" s="17"/>
+      <c r="M6" s="17">
         <v>11</v>
       </c>
-      <c r="M6" s="17">
+      <c r="N6" s="17">
         <v>3</v>
       </c>
-      <c r="N6" s="15">
+      <c r="O6" s="15">
         <v>4831.9225000000006</v>
       </c>
-      <c r="O6" s="17">
+      <c r="P6" s="17">
         <v>0.106</v>
       </c>
-      <c r="P6" s="17">
+      <c r="Q6" s="17">
         <v>0.52500000000000002</v>
       </c>
-      <c r="Q6" s="17">
+      <c r="R6" s="17">
         <v>2.9999999999999997E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:17" s="26" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" s="26" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C7" s="21" t="s">
         <v>28</v>
@@ -1458,7 +1472,7 @@
         <v>27</v>
       </c>
       <c r="I7" s="24">
-        <v>9.8000000000000007</v>
+        <v>6.34</v>
       </c>
       <c r="J7" s="25" t="s">
         <v>22</v>
@@ -1466,23 +1480,24 @@
       <c r="K7" s="24">
         <v>4.47</v>
       </c>
-      <c r="L7" s="25">
+      <c r="L7" s="24"/>
+      <c r="M7" s="25">
         <v>6.3</v>
       </c>
-      <c r="M7" s="25">
+      <c r="N7" s="25">
         <v>4</v>
       </c>
-      <c r="N7" s="22"/>
-      <c r="O7" s="24"/>
+      <c r="O7" s="22"/>
       <c r="P7" s="24"/>
       <c r="Q7" s="24"/>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R7" s="24"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="37" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" s="38" t="s">
         <v>6</v>
       </c>
@@ -1491,14 +1506,14 @@
       </c>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" s="38" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:17" ht="13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" s="38" t="s">
         <v>5</v>
       </c>
@@ -1507,7 +1522,7 @@
       </c>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" s="38" t="s">
         <v>7</v>
       </c>
@@ -1515,7 +1530,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" s="38" t="s">
         <v>2</v>
       </c>
@@ -1524,14 +1539,14 @@
       </c>
       <c r="C15" s="38"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" s="38" t="s">
         <v>12</v>
       </c>
       <c r="B16" s="38"/>
       <c r="C16" s="38"/>
     </row>
-    <row r="17" spans="1:3" ht="13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="38" t="s">
         <v>3</v>
       </c>
@@ -1540,14 +1555,14 @@
       </c>
       <c r="C17" s="1"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="38"/>
       <c r="B18" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="1:3" ht="13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="38" t="s">
         <v>1</v>
       </c>
@@ -1556,26 +1571,26 @@
       </c>
       <c r="C19" s="1"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="38" t="s">
         <v>4</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C20" s="2"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="38" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="38" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1588,38 +1603,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="27" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.26953125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.81640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="12.26953125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.26953125" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.1796875" style="3"/>
+    <col min="2" max="2" width="43.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="12.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>40</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>3</v>
@@ -1631,7 +1646,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="27" t="s">
         <v>42</v>
       </c>
@@ -1642,12 +1657,12 @@
       <c r="F3" s="28"/>
       <c r="G3" s="28"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>16</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C4" s="3">
         <v>4000</v>
@@ -1665,12 +1680,12 @@
         <v>2007000</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C5" s="3">
         <v>12</v>
@@ -1688,12 +1703,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C6" s="3">
         <v>713800</v>
@@ -1711,12 +1726,12 @@
         <v>5650000000</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C7" s="3">
         <v>8320000</v>
@@ -1734,12 +1749,12 @@
         <v>153000000000</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C8" s="3">
         <v>3.7</v>
@@ -1757,12 +1772,12 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>41</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C9" s="3">
         <v>0.37</v>
@@ -1780,18 +1795,18 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="27" t="s">
         <v>43</v>
       </c>
       <c r="B10" s="27"/>
     </row>
-    <row r="11" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="30" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B11" s="30" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C11" s="30">
         <v>0.97499999999999998</v>
@@ -1809,12 +1824,12 @@
         <v>0.99919999999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="30" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B12" s="30" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C12" s="30">
         <v>1E-4</v>
@@ -1832,9 +1847,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C13" s="3">
         <v>78</v>
@@ -1852,18 +1867,18 @@
         <v>186</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="27" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B14" s="27"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>37</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C15" s="3">
         <v>1</v>
@@ -1881,12 +1896,12 @@
         <v>0.61470000000000002</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>38</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C16" s="3">
         <v>0</v>
@@ -1904,12 +1919,12 @@
         <v>3.6999999999999998E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>46</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C17" s="3">
         <v>1</v>
@@ -1927,12 +1942,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C18" s="3">
         <v>10</v>
@@ -1950,12 +1965,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>39</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C19" s="3">
         <v>0</v>
@@ -1973,12 +1988,12 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>47</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C20" s="3">
         <v>2</v>
@@ -1996,18 +2011,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="27" t="s">
         <v>44</v>
       </c>
       <c r="B21" s="27"/>
     </row>
-    <row r="22" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="30" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B22" s="30" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C22" s="30">
         <v>1.9E-3</v>
@@ -2025,12 +2040,12 @@
         <v>1.1999999999999999E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="30" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B23" s="30" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C23" s="30">
         <v>9.9900000000000003E-2</v>
@@ -2048,12 +2063,12 @@
         <v>8.9200000000000002E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>140</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>141</v>
       </c>
       <c r="C24" s="3">
         <v>0.8</v>
@@ -2071,18 +2086,18 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="33" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B25" s="33"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>45</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C26" s="3">
         <v>1</v>
@@ -2100,12 +2115,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C27" s="3">
         <f>1-C11</f>
@@ -2128,12 +2143,12 @@
         <v>8.0000000000002292E-4</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="26" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B28" s="26" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C28" s="26">
         <f>1-C12</f>
@@ -2167,278 +2182,282 @@
   <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="92.453125" customWidth="1"/>
+    <col min="1" max="1" width="92.42578125" customWidth="1"/>
+    <col min="3" max="3" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B1" s="3"/>
     </row>
-    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C2" s="46" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="34" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="34" t="s">
         <v>85</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="34" t="s">
+      <c r="B4" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="34" t="s">
         <v>86</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="34" t="s">
+      <c r="B5" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="34" t="s">
+        <v>88</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="34" t="s">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="34" t="s">
         <v>89</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="34" t="s">
+      <c r="B7" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="34" t="s">
         <v>90</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" s="34" t="s">
+      <c r="B8" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="34" t="s">
         <v>91</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" s="34" t="s">
+      <c r="B9" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" s="34" t="s">
-        <v>93</v>
-      </c>
       <c r="B10" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="27" t="s">
         <v>43</v>
       </c>
       <c r="B11" s="27"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B14" s="3"/>
       <c r="D14" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="34" t="s">
+        <v>95</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="34" t="s">
+        <v>97</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="27" t="s">
+        <v>143</v>
+      </c>
+      <c r="B23" s="3"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15" s="34" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="B27" s="3"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="B32" s="26" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="35" t="s">
+        <v>105</v>
+      </c>
+      <c r="B33" s="36"/>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16" s="34" t="s">
+      <c r="B34" s="3"/>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
         <v>98</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A19" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A20" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A21" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A22" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A23" s="27" t="s">
-        <v>144</v>
-      </c>
-      <c r="B23" s="3"/>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A24" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A25" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A26" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A27" s="27" t="s">
-        <v>76</v>
-      </c>
-      <c r="B27" s="3"/>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A28" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A29" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A30" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A31" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="26" t="s">
-        <v>107</v>
-      </c>
-      <c r="B32" s="26" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A33" s="35" t="s">
-        <v>106</v>
-      </c>
-      <c r="B33" s="36"/>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A34" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="B34" s="3"/>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A35" s="3" t="s">
-        <v>99</v>
       </c>
       <c r="B35" s="3"/>
     </row>
@@ -2450,66 +2469,66 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M16"/>
+  <dimension ref="A1:M39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="6" width="9.1796875" style="3"/>
+    <col min="1" max="6" width="9.140625" style="3"/>
     <col min="7" max="7" width="10" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.1796875" style="3"/>
+    <col min="8" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="D2" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="E2" s="6" t="s">
+      <c r="G2" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="K2" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="F2" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="G2" s="12" t="s">
-        <v>142</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="J2" s="6" t="s">
+      <c r="L2" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="M2" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="K2" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
@@ -2548,9 +2567,9 @@
         <v>-16.721576535678501</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B4" s="43">
         <v>64.278501302969502</v>
@@ -2587,7 +2606,7 @@
         <v>-59.441311511547198</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -2626,7 +2645,7 @@
         <v>-172.326708872983</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>1</v>
       </c>
@@ -2665,7 +2684,7 @@
         <v>-4.0844277396896604</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
         <v>4</v>
       </c>
@@ -2704,16 +2723,16 @@
         <v>-12.472627737519201</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="B9"/>
       <c r="C9"/>
       <c r="D9"/>
       <c r="E9"/>
       <c r="F9"/>
     </row>
-    <row r="10" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B10"/>
       <c r="C10"/>
@@ -2721,28 +2740,28 @@
       <c r="E10"/>
       <c r="F10"/>
     </row>
-    <row r="11" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B11" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="D11" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="F11" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="D11" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>74</v>
-      </c>
       <c r="G11" s="45"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>5</v>
       </c>
@@ -2767,9 +2786,9 @@
         <v>-0.23160105405480638</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B13" s="43">
         <f>B4/$G$4</f>
@@ -2792,7 +2811,7 @@
         <v>-0.49947148531324281</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>3</v>
       </c>
@@ -2817,7 +2836,7 @@
         <v>-0.62015387135968725</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>1</v>
       </c>
@@ -2842,7 +2861,7 @@
         <v>-9.5370918574387412E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="26" t="s">
         <v>4</v>
       </c>
@@ -2867,6 +2886,7 @@
         <v>-0.18392225304194718</v>
       </c>
     </row>
+    <row r="39" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2881,25 +2901,25 @@
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="40" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="40" t="s">
+        <v>128</v>
+      </c>
+      <c r="C2" s="40" t="s">
         <v>129</v>
       </c>
-      <c r="C2" s="40" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -2910,9 +2930,9 @@
         <v>1.52</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B4" s="41">
         <v>0.68</v>
@@ -2921,7 +2941,7 @@
         <v>1.75</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -2932,7 +2952,7 @@
         <v>1.18</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -2943,7 +2963,7 @@
         <v>0.76</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="39" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
updated TP, chla, secchi, and swDOC in table
</commit_message>
<xml_diff>
--- a/Tables_SOS.xlsx
+++ b/Tables_SOS.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="156">
   <si>
     <t>Lake</t>
   </si>
@@ -653,6 +653,9 @@
   </si>
   <si>
     <t>ChlA</t>
+  </si>
+  <si>
+    <t>SW DOC (g/m3)</t>
   </si>
 </sst>
 </file>
@@ -778,7 +781,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -870,6 +873,21 @@
     <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -930,7 +948,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -965,7 +983,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1150,10 +1168,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R22"/>
+  <dimension ref="A1:S22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1169,20 +1187,20 @@
     <col min="9" max="9" width="11.42578125" style="3" customWidth="1"/>
     <col min="10" max="10" width="11.28515625" style="3" customWidth="1"/>
     <col min="11" max="12" width="7.140625" style="3" customWidth="1"/>
-    <col min="13" max="13" width="8.5703125" style="3" customWidth="1"/>
-    <col min="14" max="14" width="6.7109375" style="3" customWidth="1"/>
-    <col min="15" max="15" width="24.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="8.85546875" style="3"/>
+    <col min="13" max="14" width="8.5703125" style="3" customWidth="1"/>
+    <col min="15" max="15" width="6.7109375" style="3" customWidth="1"/>
+    <col min="16" max="16" width="24.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="8.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:18" s="12" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" s="12" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -1223,22 +1241,25 @@
         <v>153</v>
       </c>
       <c r="N2" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="O2" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="O2" s="10" t="s">
+      <c r="P2" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="P2" s="11" t="s">
+      <c r="Q2" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="Q2" s="11" t="s">
+      <c r="R2" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="R2" s="11" t="s">
+      <c r="S2" s="11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
         <v>5</v>
       </c>
@@ -1269,30 +1290,35 @@
       <c r="J3" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="K3" s="17">
-        <v>6.5</v>
-      </c>
-      <c r="L3" s="17"/>
-      <c r="M3" s="17">
-        <v>5</v>
-      </c>
-      <c r="N3" s="17">
+      <c r="K3" s="47">
+        <v>4.4680929999999996</v>
+      </c>
+      <c r="L3" s="48">
+        <v>2.0666009999999999</v>
+      </c>
+      <c r="M3" s="48">
+        <v>6.2953239999999999</v>
+      </c>
+      <c r="N3" s="48">
+        <v>9.3538669999999993</v>
+      </c>
+      <c r="O3" s="17">
         <v>4</v>
       </c>
-      <c r="O3" s="15">
+      <c r="P3" s="15">
         <v>528.27563249500008</v>
       </c>
-      <c r="P3" s="17">
+      <c r="Q3" s="17">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="Q3" s="17">
+      <c r="R3" s="17">
         <v>0.84099999999999997</v>
       </c>
-      <c r="R3" s="17">
+      <c r="S3" s="17">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
         <v>62</v>
       </c>
@@ -1323,22 +1349,27 @@
       <c r="J4" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="K4" s="17">
-        <v>2.68</v>
-      </c>
-      <c r="L4" s="17"/>
-      <c r="M4" s="18">
-        <v>132.1</v>
-      </c>
-      <c r="N4" s="18">
+      <c r="K4" s="47">
+        <v>3.0271870000000001</v>
+      </c>
+      <c r="L4" s="48">
+        <v>9.2059099999999994</v>
+      </c>
+      <c r="M4" s="49">
+        <v>135.56549999999999</v>
+      </c>
+      <c r="N4" s="49">
+        <v>5.0944419999999999</v>
+      </c>
+      <c r="O4" s="18">
         <v>6</v>
       </c>
-      <c r="O4" s="15"/>
-      <c r="P4" s="17"/>
+      <c r="P4" s="15"/>
       <c r="Q4" s="17"/>
       <c r="R4" s="17"/>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S4" s="17"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
         <v>3</v>
       </c>
@@ -1369,30 +1400,35 @@
       <c r="J5" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="K5" s="17">
-        <v>4.75</v>
-      </c>
-      <c r="L5" s="17"/>
-      <c r="M5" s="17">
-        <v>2</v>
-      </c>
-      <c r="N5" s="19">
+      <c r="K5" s="47">
+        <v>4.5320900000000002</v>
+      </c>
+      <c r="L5" s="48">
+        <v>1.4116029999999999</v>
+      </c>
+      <c r="M5" s="48">
+        <v>3.787623</v>
+      </c>
+      <c r="N5" s="48">
+        <v>7.7224019999999998</v>
+      </c>
+      <c r="O5" s="19">
         <v>5</v>
       </c>
-      <c r="O5" s="15">
+      <c r="P5" s="15">
         <v>6752.4100000000008</v>
       </c>
-      <c r="P5" s="17">
+      <c r="Q5" s="17">
         <v>0.504</v>
-      </c>
-      <c r="Q5" s="17">
-        <v>0</v>
       </c>
       <c r="R5" s="17">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S5" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
         <v>1</v>
       </c>
@@ -1423,30 +1459,35 @@
       <c r="J6" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="K6" s="17">
-        <v>5.32</v>
-      </c>
-      <c r="L6" s="17"/>
-      <c r="M6" s="17">
-        <v>11</v>
-      </c>
-      <c r="N6" s="17">
+      <c r="K6" s="47">
+        <v>5.3249639999999996</v>
+      </c>
+      <c r="L6" s="48">
+        <v>2.234003</v>
+      </c>
+      <c r="M6" s="48">
+        <v>10.98129</v>
+      </c>
+      <c r="N6" s="48">
+        <v>5.1144499999999997</v>
+      </c>
+      <c r="O6" s="17">
         <v>3</v>
       </c>
-      <c r="O6" s="15">
+      <c r="P6" s="15">
         <v>4831.9225000000006</v>
       </c>
-      <c r="P6" s="17">
+      <c r="Q6" s="17">
         <v>0.106</v>
       </c>
-      <c r="Q6" s="17">
+      <c r="R6" s="17">
         <v>0.52500000000000002</v>
       </c>
-      <c r="R6" s="17">
+      <c r="S6" s="17">
         <v>2.9999999999999997E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:18" s="26" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" s="26" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>4</v>
       </c>
@@ -1477,27 +1518,32 @@
       <c r="J7" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="K7" s="24">
-        <v>4.47</v>
-      </c>
-      <c r="L7" s="24"/>
-      <c r="M7" s="25">
-        <v>6.3</v>
-      </c>
-      <c r="N7" s="25">
+      <c r="K7" s="47">
+        <v>4.4680929999999996</v>
+      </c>
+      <c r="L7" s="50">
+        <v>2.0666009999999999</v>
+      </c>
+      <c r="M7" s="51">
+        <v>6.2953239999999999</v>
+      </c>
+      <c r="N7" s="51">
+        <v>9.3538669999999993</v>
+      </c>
+      <c r="O7" s="25">
         <v>4</v>
       </c>
-      <c r="O7" s="22"/>
-      <c r="P7" s="24"/>
+      <c r="P7" s="22"/>
       <c r="Q7" s="24"/>
       <c r="R7" s="24"/>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S7" s="24"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" s="37" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" s="38" t="s">
         <v>6</v>
       </c>
@@ -1506,14 +1552,14 @@
       </c>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12" s="38" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13" s="38" t="s">
         <v>5</v>
       </c>
@@ -1522,7 +1568,7 @@
       </c>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14" s="38" t="s">
         <v>7</v>
       </c>
@@ -1530,7 +1576,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15" s="38" t="s">
         <v>2</v>
       </c>
@@ -1539,7 +1585,7 @@
       </c>
       <c r="C15" s="38"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16" s="38" t="s">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
numbered equations in table
</commit_message>
<xml_diff>
--- a/Tables_SOS.xlsx
+++ b/Tables_SOS.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17960" windowHeight="9390" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17960" windowHeight="9390" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="1) Lake characteristics" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="169">
   <si>
     <t>Lake</t>
   </si>
@@ -400,54 +400,21 @@
     <t>g/m2/yr</t>
   </si>
   <si>
-    <t>POC Aerial = AerialLoad * Perimeter</t>
-  </si>
-  <si>
     <t>g/d</t>
   </si>
   <si>
-    <t>DOC Wetland = PropWetland * WetlandLoad * Perimeter</t>
-  </si>
-  <si>
-    <t>DOC GW = groundwater concentration * groundwater inflow rate * 86400</t>
-  </si>
-  <si>
-    <t>DOC SW =  surface water concentration * surface water inflow rate * 86400</t>
-  </si>
-  <si>
     <t>m3/d</t>
   </si>
   <si>
-    <t>Daily precipitation = rainfall * 0.001 * Area</t>
-  </si>
-  <si>
-    <t>DOC precipitation = DOC_precip * Daily precipitation</t>
-  </si>
-  <si>
-    <t>Inflow load DOC = DOC Wetland + DOC GW + DOC SW + DOC precipitation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Internal load POC = (DOC Wetland + DOC SW) * 0.1  </t>
-  </si>
-  <si>
-    <t>Inflow load POC = POC Aerial + Internal load POC</t>
-  </si>
-  <si>
     <t>GPP and Respiration</t>
   </si>
   <si>
     <t>mg/m2/d</t>
   </si>
   <si>
-    <t xml:space="preserve">GPP DOC rate = GPP rate * (GPP percent DOC/100) </t>
-  </si>
-  <si>
     <t>%</t>
   </si>
   <si>
-    <t>GPP POC rate = GPP rate * (1-(GPP percent DOC/100))</t>
-  </si>
-  <si>
     <t>g/m3</t>
   </si>
   <si>
@@ -517,15 +484,6 @@
     <t>NEP and Oxygen Flux</t>
   </si>
   <si>
-    <t>Fatm = 0.7 * (DOconc - DOsat)/Zmix</t>
-  </si>
-  <si>
-    <t>DO(t+1) = DOconc + NEP - Fatm</t>
-  </si>
-  <si>
-    <t>NEP (as O2) = (NPP - DOCrespired) * 32/12</t>
-  </si>
-  <si>
     <t>g O2/m3/d</t>
   </si>
   <si>
@@ -541,12 +499,6 @@
     <t>WetlandLoad (g/d)</t>
   </si>
   <si>
-    <t>Heterotrophic respiration of allochthonous DOC</t>
-  </si>
-  <si>
-    <t>Heterotrophic respiration of autochthonous DOC</t>
-  </si>
-  <si>
     <t>AerialLoad (g/d)</t>
   </si>
   <si>
@@ -575,9 +527,6 @@
   </si>
   <si>
     <t>MAR = mass accumulation rate</t>
-  </si>
-  <si>
-    <t>Fatm = atmospheric deposition</t>
   </si>
   <si>
     <t>Export</t>
@@ -622,42 +571,6 @@
     <t>Burial_autoch</t>
   </si>
   <si>
-    <t>Respiration_alloch</t>
-  </si>
-  <si>
-    <t>Respiration_autoch</t>
-  </si>
-  <si>
-    <t>NPP DOC_autoch = GPP DOC_autoch * 0.2 * Area / 1000</t>
-  </si>
-  <si>
-    <t>NPP POC_autoch = GPP POC_autoch * 0.2 * Area / 1000</t>
-  </si>
-  <si>
-    <t>Autochthonous Respiration = GPP DOC rate * Respiration_autoch(1.08^(epilimnion temp - 20))</t>
-  </si>
-  <si>
-    <t>MAR_autoch = POC mass * Burial_autoch * 365/Area</t>
-  </si>
-  <si>
-    <t>POC Burial_autoch = MAR_autoch * (1/365) * Area</t>
-  </si>
-  <si>
-    <t>DOC_autoch leached in = POC_autoch leached out</t>
-  </si>
-  <si>
-    <t>Allochthonous Respiration = GPP DOC rate * Respiration_alloch(1.08^(epilimnion temp - 20))</t>
-  </si>
-  <si>
-    <t>MAR_alloch = POC mass * Burial_alloch * 365/Area</t>
-  </si>
-  <si>
-    <t>POC Burial_alloch = MAR_alloch * (1/365) * Area</t>
-  </si>
-  <si>
-    <t>DOC_alloch leached in = POC_alloch leached out</t>
-  </si>
-  <si>
     <t>Hanson et al. 2014</t>
   </si>
   <si>
@@ -670,12 +583,6 @@
     <t>1.08 cited in Resp function as Hanson personal comm. Do we have anything else?</t>
   </si>
   <si>
-    <t>GPP rate  = 10^(1.18 + (0.92 * log10(chlorophyll-a * photic depth)) + (0.014 * epilimnion temperature))</t>
-  </si>
-  <si>
-    <t>GPP percent DOC = 71.4 * (chlorophyll-a * photic depth)^(-0.22)</t>
-  </si>
-  <si>
     <t>Proportion of total load</t>
   </si>
   <si>
@@ -694,16 +601,133 @@
     <t>* root mean square error (mg/L)</t>
   </si>
   <si>
-    <t>POC_alloch leached out = POC_alloch concentration * POClc_alloch * Volume</t>
-  </si>
-  <si>
-    <t>POC_autoch leached out = POC_autoch concentration * POClc_autoch * Volume</t>
-  </si>
-  <si>
-    <t>POClc alloch</t>
-  </si>
-  <si>
-    <t>POClc autoch</t>
+    <t>1a) DOC Wetland = PropWetland * WetlandLoad * Perimeter</t>
+  </si>
+  <si>
+    <t>1b) DOC GW = groundwater concentration * groundwater inflow rate * 86400</t>
+  </si>
+  <si>
+    <t>1c) DOC SW =  surface water concentration * surface water inflow rate * 86400</t>
+  </si>
+  <si>
+    <t>1d) Daily precipitation = rainfall * 0.001 * Area</t>
+  </si>
+  <si>
+    <t>1e) DOC precipitation = DOC_precip * Daily precipitation</t>
+  </si>
+  <si>
+    <t>1f) Inflow load DOC = DOC Wetland + DOC GW + DOC SW + DOC precipitation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1g) Internal load POC = (DOC Wetland + DOC SW) * 0.1  </t>
+  </si>
+  <si>
+    <t>1h) Inflow load POC = POC Aerial + Internal load POC</t>
+  </si>
+  <si>
+    <t>2a) GPP rate  = 10^(1.18 + (0.92 * log10(chlorophyll-a * photic depth)) + (0.014 * epilimnion temperature))</t>
+  </si>
+  <si>
+    <t>2b) GPP percent DOC = 71.4 * (chlorophyll-a * photic depth)^(-0.22)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2c) GPP DOC rate = GPP rate * (GPP percent DOC/100) </t>
+  </si>
+  <si>
+    <t>2d) GPP POC rate = GPP rate * (1-(GPP percent DOC/100))</t>
+  </si>
+  <si>
+    <t>2e) NPP DOC_autoch = GPP DOC_autoch * 0.2 * Area / 1000</t>
+  </si>
+  <si>
+    <t>2f) NPP POC_autoch = GPP POC_autoch * 0.2 * Area / 1000</t>
+  </si>
+  <si>
+    <t>2g) Autochthonous Respiration = GPP DOC rate * Respiration_autoch(1.08^(epilimnion temp - 20))</t>
+  </si>
+  <si>
+    <t>2h) Allochthonous Respiration = GPP DOC rate * Respiration_alloch(1.08^(epilimnion temp - 20))</t>
+  </si>
+  <si>
+    <t>3a) MAR_alloch = POC mass * Burial_alloch * 365/Area</t>
+  </si>
+  <si>
+    <t>3b) POC Burial_alloch = MAR_alloch * (1/365) * Area</t>
+  </si>
+  <si>
+    <t>3c) MAR_autoch = POC mass * Burial_autoch * 365/Area</t>
+  </si>
+  <si>
+    <t>3d) POC Burial_autoch = MAR_autoch * (1/365) * Area</t>
+  </si>
+  <si>
+    <t>4a) NEP (as O2) = (NPP - DOCrespired) * 32/12</t>
+  </si>
+  <si>
+    <t>4b) Fatm = 0.7 * (DOconc - DOsat)/Zmix</t>
+  </si>
+  <si>
+    <t>4c) DO(t+1) = DOconc + NEP - Fatm</t>
+  </si>
+  <si>
+    <t>Fatm = atmospheric flux rate</t>
+  </si>
+  <si>
+    <t>Zmix = mix depth</t>
+  </si>
+  <si>
+    <t>5a) POC Aerial = AerialLoad * Perimeter</t>
+  </si>
+  <si>
+    <t>5b) POC_alloch leached out = POC_alloch concentration * POClc_alloch * Volume</t>
+  </si>
+  <si>
+    <t>5c) POC_autoch leached out = POC_autoch concentration * POClc_autoch * Volume</t>
+  </si>
+  <si>
+    <t>5d) DOC_alloch leached in = POC_alloch leached out</t>
+  </si>
+  <si>
+    <t>5e) DOC_autoch leached in = POC_autoch leached out</t>
+  </si>
+  <si>
+    <t>POClc_autoch</t>
+  </si>
+  <si>
+    <t>POClc_alloch</t>
+  </si>
+  <si>
+    <t>Decomposition rate of allochthonous DOC in heterotrophic respiration</t>
+  </si>
+  <si>
+    <t>Decomposition rate of autochthonous DOC in heterotrophic respiration</t>
+  </si>
+  <si>
+    <r>
+      <t>Respiration_alloch (d</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>¯¹</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>Respiration_autoch (d¯¹)</t>
   </si>
 </sst>
 </file>
@@ -714,7 +738,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -798,6 +822,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -846,7 +883,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -971,6 +1008,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1322,16 +1360,16 @@
         <v>52</v>
       </c>
       <c r="L2" s="9" t="s">
-        <v>131</v>
+        <v>114</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="N2" s="7" t="s">
         <v>54</v>
       </c>
       <c r="O2" s="7" t="s">
-        <v>132</v>
+        <v>115</v>
       </c>
       <c r="P2" s="10" t="s">
         <v>19</v>
@@ -1346,7 +1384,7 @@
         <v>10</v>
       </c>
       <c r="T2" s="7" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
@@ -1393,7 +1431,7 @@
         <v>4</v>
       </c>
       <c r="O3" s="53" t="s">
-        <v>133</v>
+        <v>116</v>
       </c>
       <c r="P3" s="15">
         <v>528.27563249500008</v>
@@ -1455,7 +1493,7 @@
         <v>6</v>
       </c>
       <c r="O4" s="18" t="s">
-        <v>136</v>
+        <v>119</v>
       </c>
       <c r="P4" s="15"/>
       <c r="Q4" s="17"/>
@@ -1509,7 +1547,7 @@
         <v>5</v>
       </c>
       <c r="O5" s="18" t="s">
-        <v>135</v>
+        <v>118</v>
       </c>
       <c r="P5" s="15">
         <v>6752.4100000000008</v>
@@ -1571,7 +1609,7 @@
         <v>3</v>
       </c>
       <c r="O6" s="53" t="s">
-        <v>137</v>
+        <v>120</v>
       </c>
       <c r="P6" s="15">
         <v>4831.9225000000006</v>
@@ -1633,7 +1671,7 @@
         <v>4</v>
       </c>
       <c r="O7" s="25" t="s">
-        <v>134</v>
+        <v>117</v>
       </c>
       <c r="P7" s="22"/>
       <c r="Q7" s="24"/>
@@ -1757,8 +1795,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1774,7 +1812,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -1782,7 +1820,7 @@
         <v>40</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>5</v>
@@ -1816,7 +1854,7 @@
         <v>16</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="C4" s="3">
         <v>4000</v>
@@ -1839,7 +1877,7 @@
         <v>17</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="C5" s="3">
         <v>12</v>
@@ -1859,10 +1897,10 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="C6" s="3">
         <v>713800</v>
@@ -1885,7 +1923,7 @@
         <v>53</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="C7" s="3">
         <v>8320000</v>
@@ -1905,10 +1943,10 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="C8" s="55">
         <v>3.7</v>
@@ -1931,7 +1969,7 @@
         <v>41</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>127</v>
+        <v>111</v>
       </c>
       <c r="C9" s="55">
         <v>0.37</v>
@@ -1951,16 +1989,16 @@
     </row>
     <row r="10" spans="1:7" ht="13" x14ac:dyDescent="0.3">
       <c r="A10" s="27" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="B10" s="27"/>
     </row>
     <row r="11" spans="1:7" ht="13" x14ac:dyDescent="0.3">
       <c r="A11" s="30" t="s">
-        <v>138</v>
+        <v>121</v>
       </c>
       <c r="B11" s="30" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="C11" s="48">
         <v>1</v>
@@ -1980,10 +2018,10 @@
     </row>
     <row r="12" spans="1:7" ht="13" x14ac:dyDescent="0.3">
       <c r="A12" s="30" t="s">
-        <v>139</v>
+        <v>122</v>
       </c>
       <c r="B12" s="30" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="C12" s="48">
         <v>0</v>
@@ -2003,7 +2041,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="C13" s="3">
         <v>78</v>
@@ -2032,7 +2070,7 @@
         <v>37</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="C15" s="41">
         <v>1</v>
@@ -2055,7 +2093,7 @@
         <v>38</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="C16" s="41">
         <v>0</v>
@@ -2075,10 +2113,10 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="C17" s="3">
         <v>1</v>
@@ -2098,10 +2136,10 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="C18" s="3">
         <v>10</v>
@@ -2124,7 +2162,7 @@
         <v>39</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="C19" s="55">
         <v>0</v>
@@ -2147,7 +2185,7 @@
         <v>44</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="C20" s="3">
         <v>2</v>
@@ -2173,10 +2211,10 @@
     </row>
     <row r="22" spans="1:7" ht="13" x14ac:dyDescent="0.3">
       <c r="A22" s="30" t="s">
-        <v>140</v>
+        <v>167</v>
       </c>
       <c r="B22" s="30" t="s">
-        <v>117</v>
+        <v>165</v>
       </c>
       <c r="C22" s="48">
         <v>1.5E-3</v>
@@ -2196,10 +2234,10 @@
     </row>
     <row r="23" spans="1:7" ht="13" x14ac:dyDescent="0.3">
       <c r="A23" s="30" t="s">
-        <v>141</v>
+        <v>168</v>
       </c>
       <c r="B23" s="30" t="s">
-        <v>118</v>
+        <v>166</v>
       </c>
       <c r="C23" s="48">
         <v>9.2299999999999993E-2</v>
@@ -2219,10 +2257,10 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="C24" s="3">
         <v>0.8</v>
@@ -2248,10 +2286,10 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
       <c r="C26" s="3">
         <v>1</v>
@@ -2271,10 +2309,10 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>123</v>
+        <v>107</v>
       </c>
       <c r="C27" s="41">
         <f>1-C11</f>
@@ -2299,10 +2337,10 @@
     </row>
     <row r="28" spans="1:7" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="26" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B28" s="26" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="C28" s="42">
         <f>1-C12</f>
@@ -2333,10 +2371,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C36"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2348,7 +2386,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="B1" s="3"/>
     </row>
@@ -2360,166 +2398,166 @@
         <v>67</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="33" t="s">
-        <v>72</v>
+        <v>133</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C3" t="s">
-        <v>152</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="33" t="s">
-        <v>73</v>
+        <v>134</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C4" t="s">
-        <v>152</v>
+        <v>123</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="33" t="s">
-        <v>74</v>
+        <v>135</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C5" t="s">
-        <v>152</v>
+        <v>123</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="33" t="s">
-        <v>76</v>
+        <v>136</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C6" t="s">
-        <v>152</v>
+        <v>123</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="33" t="s">
-        <v>77</v>
+        <v>137</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C7" t="s">
-        <v>152</v>
+        <v>123</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="33" t="s">
-        <v>78</v>
+        <v>138</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C8" t="s">
-        <v>152</v>
+        <v>123</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="33" t="s">
-        <v>79</v>
+        <v>139</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C9" t="s">
-        <v>152</v>
+        <v>123</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="33" t="s">
-        <v>80</v>
+        <v>140</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C10" t="s">
-        <v>152</v>
+        <v>123</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="27" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="B11" s="3"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="33" t="s">
-        <v>156</v>
+        <v>141</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="C12" t="s">
-        <v>153</v>
+        <v>124</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="33" t="s">
-        <v>157</v>
+        <v>142</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="C13" t="s">
-        <v>154</v>
+        <v>125</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
-        <v>83</v>
+        <v>143</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
-        <v>85</v>
+        <v>144</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C18" t="s">
-        <v>155</v>
+        <v>126</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
@@ -2527,12 +2565,12 @@
         <v>148</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="27" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="B20" s="27"/>
     </row>
@@ -2549,12 +2587,12 @@
         <v>150</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>69</v>
@@ -2562,40 +2600,40 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
-        <v>146</v>
+        <v>152</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="27" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="B25" s="3"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
-        <v>111</v>
+        <v>153</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
-        <v>109</v>
+        <v>154</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
-        <v>110</v>
+        <v>155</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
@@ -2606,59 +2644,64 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
-        <v>70</v>
+        <v>158</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>68</v>
       </c>
       <c r="C30" t="s">
-        <v>152</v>
+        <v>123</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
-        <v>151</v>
+        <v>161</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="26" t="s">
-        <v>147</v>
+        <v>162</v>
       </c>
       <c r="B34" s="26" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C34" s="37"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="34" t="s">
-        <v>128</v>
+        <v>112</v>
       </c>
       <c r="B35" s="34"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="34" t="s">
-        <v>129</v>
+        <v>156</v>
       </c>
       <c r="B36" s="34"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A37" s="60" t="s">
+        <v>157</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2697,16 +2740,16 @@
         <v>63</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>130</v>
+        <v>113</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -2831,7 +2874,7 @@
     </row>
     <row r="9" spans="1:7" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A9" s="57" t="s">
-        <v>158</v>
+        <v>127</v>
       </c>
       <c r="B9"/>
       <c r="C9"/>
@@ -2984,7 +3027,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>159</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2992,10 +3035,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="38" t="s">
-        <v>160</v>
+        <v>129</v>
       </c>
       <c r="C2" s="38" t="s">
-        <v>161</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -3055,12 +3098,12 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="59" t="s">
-        <v>163</v>
+        <v>132</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="59" t="s">
-        <v>162</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
first year model artifact removal
</commit_message>
<xml_diff>
--- a/Tables_SOS.xlsx
+++ b/Tables_SOS.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17830"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\immcc\Desktop\SOS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Ian_GIS\gleon\SOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17960" windowHeight="9390" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17955" windowHeight="9390" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="1) Lake characteristics" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="4) Model fits" sheetId="5" r:id="rId4"/>
     <sheet name="5) Mass balances" sheetId="4" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -766,7 +766,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -1338,36 +1338,36 @@
       <selection sqref="A1:O7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.36328125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="14.54296875" style="4" customWidth="1"/>
-    <col min="3" max="3" width="13.453125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.42578125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.81640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.6328125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.08984375" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.26953125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.90625" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="7.1796875" style="3" customWidth="1"/>
-    <col min="13" max="13" width="8.54296875" style="3" customWidth="1"/>
-    <col min="14" max="14" width="6.7265625" style="3" customWidth="1"/>
-    <col min="15" max="15" width="21.1796875" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="24.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.81640625" style="3"/>
-    <col min="20" max="20" width="8.54296875" style="3" customWidth="1"/>
-    <col min="21" max="16384" width="8.81640625" style="3"/>
+    <col min="5" max="5" width="6.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="7.140625" style="3" customWidth="1"/>
+    <col min="13" max="13" width="8.5703125" style="3" customWidth="1"/>
+    <col min="14" max="14" width="6.7109375" style="3" customWidth="1"/>
+    <col min="15" max="15" width="21.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="24.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.85546875" style="3"/>
+    <col min="20" max="20" width="8.5703125" style="3" customWidth="1"/>
+    <col min="21" max="16384" width="8.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" ht="12.95" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:20" s="12" customFormat="1" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:20" s="12" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -1429,7 +1429,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
         <v>5</v>
       </c>
@@ -1491,7 +1491,7 @@
         <v>6.2953239999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
         <v>58</v>
       </c>
@@ -1545,7 +1545,7 @@
         <v>135.56549999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
         <v>3</v>
       </c>
@@ -1607,7 +1607,7 @@
         <v>3.787623</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="26.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" ht="26.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
         <v>1</v>
       </c>
@@ -1669,7 +1669,7 @@
         <v>10.98129</v>
       </c>
     </row>
-    <row r="7" spans="1:20" s="26" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" s="26" customFormat="1" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
         <v>4</v>
       </c>
@@ -1723,12 +1723,12 @@
         <v>6.2953239999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" ht="12.6" x14ac:dyDescent="0.25">
       <c r="A10" s="34" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" s="35" t="s">
         <v>6</v>
       </c>
@@ -1737,14 +1737,14 @@
       </c>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" ht="12.6" x14ac:dyDescent="0.25">
       <c r="A12" s="35" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:20" ht="13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13" s="35" t="s">
         <v>5</v>
       </c>
@@ -1753,7 +1753,7 @@
       </c>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" ht="12.6" x14ac:dyDescent="0.25">
       <c r="A14" s="35" t="s">
         <v>7</v>
       </c>
@@ -1761,7 +1761,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" ht="12.6" x14ac:dyDescent="0.25">
       <c r="A15" s="35" t="s">
         <v>2</v>
       </c>
@@ -1770,14 +1770,14 @@
       </c>
       <c r="C15" s="35"/>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" ht="12.6" x14ac:dyDescent="0.25">
       <c r="A16" s="35" t="s">
         <v>12</v>
       </c>
       <c r="B16" s="35"/>
       <c r="C16" s="35"/>
     </row>
-    <row r="17" spans="1:3" ht="13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="12.95" x14ac:dyDescent="0.25">
       <c r="A17" s="35" t="s">
         <v>3</v>
       </c>
@@ -1786,14 +1786,14 @@
       </c>
       <c r="C17" s="1"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="12.6" x14ac:dyDescent="0.25">
       <c r="A18" s="35"/>
       <c r="B18" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="1:3" ht="13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="12.95" x14ac:dyDescent="0.25">
       <c r="A19" s="35" t="s">
         <v>1</v>
       </c>
@@ -1802,7 +1802,7 @@
       </c>
       <c r="C19" s="1"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="35" t="s">
         <v>4</v>
       </c>
@@ -1811,12 +1811,12 @@
       </c>
       <c r="C20" s="2"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="12.6" x14ac:dyDescent="0.25">
       <c r="A21" s="35" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A22" s="35" t="s">
         <v>58</v>
       </c>
@@ -1841,18 +1841,18 @@
       <selection sqref="A1:G28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="25" style="3" customWidth="1"/>
-    <col min="2" max="2" width="58.08984375" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.81640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="8.81640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.81640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.6328125" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.1796875" style="3"/>
+    <col min="2" max="2" width="58.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="8.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="12.95" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>73</v>
       </c>
@@ -1880,7 +1880,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="12.95" x14ac:dyDescent="0.3">
       <c r="A3" s="27" t="s">
         <v>42</v>
       </c>
@@ -1891,7 +1891,7 @@
       <c r="F3" s="28"/>
       <c r="G3" s="28"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="12.6" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>16</v>
       </c>
@@ -1914,7 +1914,7 @@
         <v>2007000</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="12.6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>17</v>
       </c>
@@ -1937,7 +1937,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>75</v>
       </c>
@@ -1960,7 +1960,7 @@
         <v>5650000000</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>52</v>
       </c>
@@ -1983,7 +1983,7 @@
         <v>153000000000</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>76</v>
       </c>
@@ -2006,7 +2006,7 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>41</v>
       </c>
@@ -2029,13 +2029,13 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="12.95" x14ac:dyDescent="0.3">
       <c r="A10" s="27" t="s">
         <v>177</v>
       </c>
       <c r="B10" s="27"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="12.6" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>37</v>
       </c>
@@ -2058,7 +2058,7 @@
         <v>0.61470000000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="12.6" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>38</v>
       </c>
@@ -2081,7 +2081,7 @@
         <v>3.6999999999999998E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="12.6" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>97</v>
       </c>
@@ -2104,7 +2104,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>78</v>
       </c>
@@ -2127,7 +2127,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="12.6" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>39</v>
       </c>
@@ -2150,7 +2150,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>43</v>
       </c>
@@ -2173,7 +2173,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="12.6" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>98</v>
       </c>
@@ -2196,13 +2196,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" ht="12.95" x14ac:dyDescent="0.3">
       <c r="A18" s="27" t="s">
         <v>176</v>
       </c>
       <c r="B18" s="27"/>
     </row>
-    <row r="19" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="30" t="s">
         <v>145</v>
       </c>
@@ -2225,7 +2225,7 @@
         <v>1.2999999999999999E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="30" t="s">
         <v>146</v>
       </c>
@@ -2248,7 +2248,7 @@
         <v>6.8599999999999994E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="12.6" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>90</v>
       </c>
@@ -2271,13 +2271,13 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" ht="12.95" x14ac:dyDescent="0.3">
       <c r="A22" s="27" t="s">
         <v>88</v>
       </c>
       <c r="B22" s="27"/>
     </row>
-    <row r="23" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" ht="12.95" x14ac:dyDescent="0.3">
       <c r="A23" s="30" t="s">
         <v>116</v>
       </c>
@@ -2300,7 +2300,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" ht="12.95" x14ac:dyDescent="0.3">
       <c r="A24" s="30" t="s">
         <v>117</v>
       </c>
@@ -2323,7 +2323,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>77</v>
       </c>
@@ -2343,13 +2343,13 @@
         <v>186</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" ht="12.95" x14ac:dyDescent="0.3">
       <c r="A26" s="32" t="s">
         <v>63</v>
       </c>
       <c r="B26" s="32"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="12.6" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>142</v>
       </c>
@@ -2357,27 +2357,27 @@
         <v>102</v>
       </c>
       <c r="C27" s="36">
-        <f>1-C23</f>
+        <f t="shared" ref="C27:G28" si="0">1-C23</f>
         <v>0</v>
       </c>
       <c r="D27" s="36">
-        <f>1-D23</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E27" s="36">
-        <f>1-E23</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F27" s="36">
-        <f>1-F23</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G27" s="36">
-        <f>1-G23</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" ht="12.95" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="26" t="s">
         <v>141</v>
       </c>
@@ -2385,23 +2385,23 @@
         <v>103</v>
       </c>
       <c r="C28" s="37">
-        <f>1-C24</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="D28" s="37">
-        <f>1-D24</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="E28" s="37">
-        <f>1-E24</f>
+        <f t="shared" si="0"/>
         <v>3.2000000000000028E-2</v>
       </c>
       <c r="F28" s="37">
-        <f>1-F24</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G28" s="37">
-        <f>1-G24</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2415,25 +2415,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="97.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="97.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="56" t="s">
         <v>72</v>
       </c>
       <c r="B1" s="56"/>
       <c r="C1" s="56"/>
     </row>
-    <row r="2" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="57" t="s">
         <v>166</v>
       </c>
@@ -2444,7 +2444,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="58" t="s">
         <v>155</v>
       </c>
@@ -2455,7 +2455,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="58" t="s">
         <v>156</v>
       </c>
@@ -2466,7 +2466,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="58" t="s">
         <v>157</v>
       </c>
@@ -2477,7 +2477,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="58" t="s">
         <v>158</v>
       </c>
@@ -2488,7 +2488,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="58" t="s">
         <v>159</v>
       </c>
@@ -2499,7 +2499,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="58" t="s">
         <v>160</v>
       </c>
@@ -2510,7 +2510,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="58" t="s">
         <v>161</v>
       </c>
@@ -2521,7 +2521,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="58" t="s">
         <v>162</v>
       </c>
@@ -2532,7 +2532,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="58" t="s">
         <v>163</v>
       </c>
@@ -2543,7 +2543,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="56" t="s">
         <v>167</v>
       </c>
@@ -2554,14 +2554,14 @@
         <v>118</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="59" t="s">
         <v>168</v>
       </c>
       <c r="B13" s="56"/>
       <c r="C13" s="56"/>
     </row>
-    <row r="14" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="58" t="s">
         <v>127</v>
       </c>
@@ -2572,7 +2572,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="58" t="s">
         <v>128</v>
       </c>
@@ -2583,7 +2583,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="56" t="s">
         <v>129</v>
       </c>
@@ -2592,7 +2592,7 @@
       </c>
       <c r="C16" s="56"/>
     </row>
-    <row r="17" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="56" t="s">
         <v>130</v>
       </c>
@@ -2601,7 +2601,7 @@
       </c>
       <c r="C17" s="56"/>
     </row>
-    <row r="18" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="56" t="s">
         <v>131</v>
       </c>
@@ -2610,7 +2610,7 @@
       </c>
       <c r="C18" s="56"/>
     </row>
-    <row r="19" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="56" t="s">
         <v>132</v>
       </c>
@@ -2619,7 +2619,7 @@
       </c>
       <c r="C19" s="56"/>
     </row>
-    <row r="20" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="56" t="s">
         <v>133</v>
       </c>
@@ -2630,7 +2630,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="56" t="s">
         <v>134</v>
       </c>
@@ -2639,14 +2639,14 @@
       </c>
       <c r="C21" s="56"/>
     </row>
-    <row r="22" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="59" t="s">
         <v>88</v>
       </c>
       <c r="B22" s="59"/>
       <c r="C22" s="56"/>
     </row>
-    <row r="23" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="56" t="s">
         <v>135</v>
       </c>
@@ -2655,7 +2655,7 @@
       </c>
       <c r="C23" s="56"/>
     </row>
-    <row r="24" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="56" t="s">
         <v>164</v>
       </c>
@@ -2664,7 +2664,7 @@
       </c>
       <c r="C24" s="56"/>
     </row>
-    <row r="25" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="56" t="s">
         <v>165</v>
       </c>
@@ -2673,7 +2673,7 @@
       </c>
       <c r="C25" s="56"/>
     </row>
-    <row r="26" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="56" t="s">
         <v>136</v>
       </c>
@@ -2682,7 +2682,7 @@
       </c>
       <c r="C26" s="56"/>
     </row>
-    <row r="27" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="56" t="s">
         <v>169</v>
       </c>
@@ -2691,7 +2691,7 @@
       </c>
       <c r="C27" s="56"/>
     </row>
-    <row r="28" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="56" t="s">
         <v>170</v>
       </c>
@@ -2700,7 +2700,7 @@
       </c>
       <c r="C28" s="56"/>
     </row>
-    <row r="29" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="56" t="s">
         <v>171</v>
       </c>
@@ -2709,7 +2709,7 @@
       </c>
       <c r="C29" s="56"/>
     </row>
-    <row r="30" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="60" t="s">
         <v>172</v>
       </c>
@@ -2718,14 +2718,14 @@
       </c>
       <c r="C30" s="56"/>
     </row>
-    <row r="31" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="59" t="s">
         <v>93</v>
       </c>
       <c r="B31" s="56"/>
       <c r="C31" s="56"/>
     </row>
-    <row r="32" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="56" t="s">
         <v>137</v>
       </c>
@@ -2734,7 +2734,7 @@
       </c>
       <c r="C32" s="56"/>
     </row>
-    <row r="33" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="56" t="s">
         <v>138</v>
       </c>
@@ -2743,7 +2743,7 @@
       </c>
       <c r="C33" s="56"/>
     </row>
-    <row r="34" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="61" t="s">
         <v>139</v>
       </c>
@@ -2752,21 +2752,21 @@
       </c>
       <c r="C34" s="56"/>
     </row>
-    <row r="35" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="60" t="s">
         <v>107</v>
       </c>
       <c r="B35" s="60"/>
       <c r="C35" s="56"/>
     </row>
-    <row r="36" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="60" t="s">
         <v>140</v>
       </c>
       <c r="B36" s="60"/>
       <c r="C36" s="56"/>
     </row>
-    <row r="37" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="62" t="s">
         <v>173</v>
       </c>
@@ -2787,16 +2787,16 @@
       <selection activeCell="C9" sqref="A1:C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>178</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
     </row>
-    <row r="2" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -2807,7 +2807,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
@@ -2818,7 +2818,7 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>58</v>
       </c>
@@ -2829,7 +2829,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -2840,7 +2840,7 @@
         <v>0.79</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>1</v>
       </c>
@@ -2851,7 +2851,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="26" t="s">
         <v>4</v>
       </c>
@@ -2862,14 +2862,14 @@
         <v>0.96</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="54" t="s">
         <v>126</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="54" t="s">
         <v>125</v>
       </c>
@@ -2886,21 +2886,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="A1:G14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="6" width="9.1796875" style="3"/>
+    <col min="1" max="6" width="9.140625" style="3"/>
     <col min="7" max="7" width="10" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="14" width="9.1796875" style="3"/>
+    <col min="8" max="14" width="9.140625" style="3"/>
     <col min="15" max="15" width="10" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.90625" style="3" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.1796875" style="3"/>
+    <col min="16" max="16" width="15.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>179</v>
       </c>
@@ -2911,7 +2911,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -2958,28 +2958,28 @@
         <v>149</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="36">
-        <v>39.227373665459403</v>
+        <v>39.911058312097197</v>
       </c>
       <c r="C3" s="36">
-        <v>32.972541848402997</v>
+        <v>32.9424128896</v>
       </c>
       <c r="D3" s="36">
-        <v>-49.361781911712903</v>
+        <v>-48.759044861748599</v>
       </c>
       <c r="E3" s="36">
-        <v>-5.2397218243944401</v>
+        <v>-5.3017393251846103</v>
       </c>
       <c r="F3" s="36">
-        <v>-16.721576535678501</v>
+        <v>-17.415200198005</v>
       </c>
       <c r="G3" s="36">
         <f>SUM(B3:C3)</f>
-        <v>72.199915513862408</v>
+        <v>72.853471201697204</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>5</v>
@@ -3003,82 +3003,82 @@
         <v>154</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>58</v>
       </c>
       <c r="B4" s="36">
-        <v>64.278501302969502</v>
+        <v>66.303159712552102</v>
       </c>
       <c r="C4" s="36">
-        <v>53.989390405054699</v>
+        <v>54.7168588588939</v>
       </c>
       <c r="D4" s="36">
-        <v>-17.2970662136591</v>
+        <v>-16.5182492312344</v>
       </c>
       <c r="E4" s="36">
-        <v>-43.585940747489801</v>
+        <v>-44.3848619195685</v>
       </c>
       <c r="F4" s="36">
-        <v>-59.071439536272599</v>
+        <v>-61.055035308213</v>
       </c>
       <c r="G4" s="36">
         <f t="shared" ref="G4:G7" si="0">SUM(B4:C4)</f>
-        <v>118.26789170802419</v>
+        <v>121.020018571446</v>
       </c>
       <c r="I4" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="36">
-        <v>75.974568212740095</v>
+        <v>72.775175448556794</v>
       </c>
       <c r="C5" s="36">
-        <v>11.5887156501019</v>
+        <v>11.4771511916558</v>
       </c>
       <c r="D5" s="36">
-        <v>-24.698945130072602</v>
+        <v>-24.0331239756059</v>
       </c>
       <c r="E5" s="36">
-        <v>-6.6632551913195002</v>
+        <v>-6.3727021573982903</v>
       </c>
       <c r="F5" s="36">
-        <v>-55.798398440631402</v>
+        <v>-53.415329388723002</v>
       </c>
       <c r="G5" s="36">
         <f t="shared" si="0"/>
-        <v>87.563283862841999</v>
+        <v>84.252326640212601</v>
       </c>
       <c r="I5" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="36">
-        <v>13.767220528508201</v>
+        <v>13.769777258250601</v>
       </c>
       <c r="C6" s="36">
-        <v>29.6939341325543</v>
+        <v>28.140834484649201</v>
       </c>
       <c r="D6" s="36">
-        <v>-38.1948755798024</v>
+        <v>-37.084408704860003</v>
       </c>
       <c r="E6" s="36">
-        <v>-1.2121897918037099</v>
+        <v>-1.21205080195923</v>
       </c>
       <c r="F6" s="36">
-        <v>-4.1449302423290497</v>
+        <v>-4.1299826785709701</v>
       </c>
       <c r="G6" s="36">
         <f t="shared" si="0"/>
-        <v>43.461154661062501</v>
+        <v>41.910611742899803</v>
       </c>
       <c r="I6" s="3" t="s">
         <v>1</v>
@@ -3103,34 +3103,34 @@
         <v>150</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="53">
-        <v>40.946599812544498</v>
-      </c>
-      <c r="C7" s="53">
-        <v>26.868074764514802</v>
-      </c>
-      <c r="D7" s="53">
-        <v>-35.3411046102173</v>
-      </c>
-      <c r="E7" s="53">
-        <v>-20.5409199346328</v>
-      </c>
-      <c r="F7" s="53">
-        <v>-12.472627737519201</v>
+      <c r="B7" s="36">
+        <v>39.576465329266298</v>
+      </c>
+      <c r="C7" s="36">
+        <v>26.4145231974755</v>
+      </c>
+      <c r="D7" s="36">
+        <v>-33.375631727461503</v>
+      </c>
+      <c r="E7" s="36">
+        <v>-20.100651477426499</v>
+      </c>
+      <c r="F7" s="36">
+        <v>-12.234891490866801</v>
       </c>
       <c r="G7" s="53">
         <f t="shared" si="0"/>
-        <v>67.814674577059293</v>
+        <v>65.990988526741802</v>
       </c>
       <c r="I7" s="33" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="52" t="s">
         <v>122</v>
       </c>
@@ -3144,85 +3144,85 @@
       </c>
       <c r="J9" s="52"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B10" s="36">
         <f>B3/$G$3</f>
-        <v>0.54331606050048264</v>
+        <v>0.54782644743998721</v>
       </c>
       <c r="C10" s="36">
         <f t="shared" ref="C10:F10" si="1">C3/$G$3</f>
-        <v>0.45668393949951724</v>
+        <v>0.45217355256001268</v>
       </c>
       <c r="D10" s="36">
         <f>D3/$G$3</f>
-        <v>-0.68368198993578355</v>
+        <v>-0.66927552054119144</v>
       </c>
       <c r="E10" s="36">
         <f t="shared" si="1"/>
-        <v>-7.2572409359515269E-2</v>
+        <v>-7.2772638526811886E-2</v>
       </c>
       <c r="F10" s="36">
         <f t="shared" si="1"/>
-        <v>-0.23160105405480638</v>
+        <v>-0.23904420627797476</v>
       </c>
       <c r="I10" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>58</v>
       </c>
       <c r="B11" s="36">
         <f>B4/$G$4</f>
-        <v>0.54349917272270409</v>
+        <v>0.54786935661730229</v>
       </c>
       <c r="C11" s="36">
         <f t="shared" ref="C11:F11" si="2">C4/$G$4</f>
-        <v>0.45650082727729596</v>
+        <v>0.45213064338269765</v>
       </c>
       <c r="D11" s="36">
         <f t="shared" si="2"/>
-        <v>-0.14625327266644372</v>
+        <v>-0.13649187486682296</v>
       </c>
       <c r="E11" s="36">
         <f t="shared" si="2"/>
-        <v>-0.36853570413763109</v>
+        <v>-0.36675636348018925</v>
       </c>
       <c r="F11" s="36">
         <f t="shared" si="2"/>
-        <v>-0.49947148531324281</v>
+        <v>-0.50450360220502066</v>
       </c>
       <c r="I11" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B12" s="36">
         <f>B5/$G$5</f>
-        <v>0.86765325443647912</v>
+        <v>0.86377644808947152</v>
       </c>
       <c r="C12" s="36">
         <f t="shared" ref="C12:F12" si="3">C5/$G$5</f>
-        <v>0.13234674556352083</v>
+        <v>0.13622355191052846</v>
       </c>
       <c r="D12" s="36">
         <f t="shared" si="3"/>
-        <v>-0.2820696534035968</v>
+        <v>-0.28525175427185395</v>
       </c>
       <c r="E12" s="36">
         <f t="shared" si="3"/>
-        <v>-7.6096451587593927E-2</v>
+        <v>-7.5638292870082918E-2</v>
       </c>
       <c r="F12" s="36">
         <f t="shared" si="3"/>
-        <v>-0.63723510561839247</v>
+        <v>-0.6339923361027815</v>
       </c>
       <c r="I12" s="3" t="s">
         <v>3</v>
@@ -3237,29 +3237,29 @@
         <v>153</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B13" s="36">
         <f>B6/$G$6</f>
-        <v>0.31677070330674989</v>
+        <v>0.32855109208906685</v>
       </c>
       <c r="C13" s="36">
         <f t="shared" ref="C13:F13" si="4">C6/$G$6</f>
-        <v>0.68322929669325005</v>
+        <v>0.67144890791093303</v>
       </c>
       <c r="D13" s="36">
         <f t="shared" si="4"/>
-        <v>-0.87882790684394219</v>
+        <v>-0.88484532109323311</v>
       </c>
       <c r="E13" s="36">
         <f t="shared" si="4"/>
-        <v>-2.7891338857817527E-2</v>
+        <v>-2.8919902419810586E-2</v>
       </c>
       <c r="F13" s="36">
         <f t="shared" si="4"/>
-        <v>-9.5370918574387412E-2</v>
+        <v>-9.8542648432485419E-2</v>
       </c>
       <c r="I13" s="3" t="s">
         <v>1</v>
@@ -3277,36 +3277,36 @@
         <v>0.31092964824120606</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="26" t="s">
         <v>4</v>
       </c>
       <c r="B14" s="37">
         <f>B7/$G$7</f>
-        <v>0.60380146432784232</v>
+        <v>0.59972529905698513</v>
       </c>
       <c r="C14" s="37">
         <f t="shared" ref="C14:F14" si="5">C7/$G$7</f>
-        <v>0.39619853567215785</v>
+        <v>0.40027470094301487</v>
       </c>
       <c r="D14" s="37">
         <f t="shared" si="5"/>
-        <v>-0.52114243459294984</v>
+        <v>-0.50576044506344309</v>
       </c>
       <c r="E14" s="37">
         <f t="shared" si="5"/>
-        <v>-0.30289786189701029</v>
+        <v>-0.30459691430870184</v>
       </c>
       <c r="F14" s="37">
         <f t="shared" si="5"/>
-        <v>-0.18392225304194718</v>
+        <v>-0.18540245818425352</v>
       </c>
       <c r="G14" s="26"/>
       <c r="I14" s="26" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="37" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" ht="8.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>